<commit_message>
Results missing personality 0200
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tudublin-my.sharepoint.com/personal/lucas_rizzo_tudublin_ie/Documents/rulex/Multiclass/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="657" documentId="11_AD4DB114E441178AC67DF4065653DB7A683EDF12" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F08B9F6-66B8-4BEC-A6FB-7AA7A126676D}"/>
+  <xr:revisionPtr revIDLastSave="691" documentId="11_AD4DB114E441178AC67DF4065653DB7A683EDF12" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0D6743E-6A2D-47FD-9E22-9517CCF1BE9E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="52">
   <si>
     <t>Data</t>
   </si>
@@ -236,12 +236,15 @@
   <si>
     <t>β</t>
   </si>
+  <si>
+    <t>nan</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,6 +271,12 @@
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -302,7 +311,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -445,11 +454,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </right>
+      <top style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -462,16 +495,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -490,29 +537,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1191,8 +1228,8 @@
   <dimension ref="A1:AN35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
+      <pane ySplit="2" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1204,15 +1241,15 @@
     <col min="5" max="5" width="19.28515625" customWidth="1"/>
     <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.5703125" customWidth="1"/>
-    <col min="8" max="8" width="24.42578125" style="13" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" style="22" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" style="22" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" style="22" customWidth="1"/>
-    <col min="12" max="12" width="6.28515625" style="22" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" style="22" customWidth="1"/>
-    <col min="14" max="14" width="11.140625" style="22" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" style="22" customWidth="1"/>
-    <col min="16" max="16" width="6.140625" style="22" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" style="11" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" customWidth="1"/>
+    <col min="12" max="12" width="6.28515625" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" customWidth="1"/>
+    <col min="16" max="16" width="6.140625" customWidth="1"/>
     <col min="17" max="17" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="18.140625" bestFit="1" customWidth="1"/>
@@ -1239,124 +1276,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="I1" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="30" t="s">
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="16" t="s">
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="R1" s="16"/>
-      <c r="S1" s="14" t="s">
+      <c r="R1" s="24"/>
+      <c r="S1" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="T1" s="16"/>
-      <c r="U1" s="14" t="s">
+      <c r="T1" s="24"/>
+      <c r="U1" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="V1" s="15"/>
-      <c r="W1" s="14" t="s">
+      <c r="V1" s="23"/>
+      <c r="W1" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="X1" s="16"/>
-      <c r="Y1" s="14" t="s">
+      <c r="X1" s="24"/>
+      <c r="Y1" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="Z1" s="16"/>
-      <c r="AA1" s="14" t="s">
+      <c r="Z1" s="24"/>
+      <c r="AA1" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="15"/>
-      <c r="AC1" s="14" t="s">
+      <c r="AB1" s="23"/>
+      <c r="AC1" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="16"/>
-      <c r="AE1" s="14" t="s">
+      <c r="AD1" s="24"/>
+      <c r="AE1" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="AF1" s="16"/>
-      <c r="AG1" s="14" t="s">
+      <c r="AF1" s="24"/>
+      <c r="AG1" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="AH1" s="15"/>
-      <c r="AI1" s="14" t="s">
+      <c r="AH1" s="23"/>
+      <c r="AI1" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="AJ1" s="16"/>
-      <c r="AK1" s="14" t="s">
+      <c r="AJ1" s="24"/>
+      <c r="AK1" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="AL1" s="16"/>
-      <c r="AM1" s="14" t="s">
+      <c r="AL1" s="24"/>
+      <c r="AM1" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="AN1" s="15"/>
+      <c r="AN1" s="23"/>
     </row>
     <row r="2" spans="1:40" s="3" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="23" t="s">
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="I2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="J2" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="28" t="s">
+      <c r="K2" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="L2" s="28" t="s">
+      <c r="L2" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="M2" s="31" t="s">
+      <c r="M2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="31" t="s">
+      <c r="N2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="31" t="s">
+      <c r="O2" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="P2" s="31" t="s">
+      <c r="P2" s="20" t="s">
         <v>50</v>
       </c>
       <c r="Q2" s="4" t="s">
@@ -1454,103 +1491,103 @@
       <c r="G3">
         <v>103</v>
       </c>
-      <c r="H3" s="24">
+      <c r="H3" s="15">
         <v>0.77100000000000002</v>
       </c>
-      <c r="I3" s="29">
+      <c r="I3" s="19">
         <v>1</v>
       </c>
-      <c r="J3" s="29">
+      <c r="J3" s="19">
         <v>0.26</v>
       </c>
-      <c r="K3" s="29" t="s">
+      <c r="K3" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="L3" s="29">
+      <c r="L3" s="19">
         <v>100</v>
       </c>
-      <c r="M3" s="32">
+      <c r="M3" s="21">
         <v>0.86</v>
       </c>
-      <c r="N3" s="32">
+      <c r="N3" s="21">
         <v>0.09</v>
       </c>
-      <c r="O3" s="32" t="s">
+      <c r="O3" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="P3" s="32">
+      <c r="P3" s="21">
         <v>25</v>
       </c>
-      <c r="Q3" s="21">
+      <c r="Q3" s="13">
         <v>0.86</v>
       </c>
-      <c r="R3" s="21">
+      <c r="R3" s="13">
         <v>0.09</v>
       </c>
-      <c r="S3" s="21">
+      <c r="S3" s="13">
         <v>0.86</v>
       </c>
-      <c r="T3" s="21">
+      <c r="T3" s="13">
         <v>0.09</v>
       </c>
-      <c r="U3" s="21">
+      <c r="U3" s="13">
         <v>0.86</v>
       </c>
-      <c r="V3" s="21">
+      <c r="V3" s="13">
         <v>0.09</v>
       </c>
-      <c r="W3" s="21">
+      <c r="W3" s="13">
         <v>0.76</v>
       </c>
-      <c r="X3" s="21">
+      <c r="X3" s="13">
         <v>0</v>
       </c>
-      <c r="Y3" s="21">
+      <c r="Y3" s="13">
         <v>0.76</v>
       </c>
-      <c r="Z3" s="21">
+      <c r="Z3" s="13">
         <v>0</v>
       </c>
-      <c r="AA3" s="21">
+      <c r="AA3" s="13">
         <v>0.76</v>
       </c>
-      <c r="AB3" s="21">
+      <c r="AB3" s="13">
         <v>0</v>
       </c>
-      <c r="AC3" s="21">
+      <c r="AC3" s="13">
         <v>0.76</v>
       </c>
-      <c r="AD3" s="21">
+      <c r="AD3" s="13">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AE3" s="21">
+      <c r="AE3" s="13">
         <v>0.76</v>
       </c>
-      <c r="AF3" s="21">
+      <c r="AF3" s="13">
         <v>0.06</v>
       </c>
-      <c r="AG3" s="21">
+      <c r="AG3" s="13">
         <v>0.88</v>
       </c>
-      <c r="AH3" s="21">
+      <c r="AH3" s="13">
         <v>0.15</v>
       </c>
-      <c r="AI3" s="21">
+      <c r="AI3" s="13">
         <v>0.85</v>
       </c>
-      <c r="AJ3" s="21">
+      <c r="AJ3" s="13">
         <v>0.15</v>
       </c>
-      <c r="AK3" s="21">
+      <c r="AK3" s="13">
         <v>0.84</v>
       </c>
-      <c r="AL3" s="21">
+      <c r="AL3" s="13">
         <v>0.14000000000000001</v>
       </c>
-      <c r="AM3" s="21">
+      <c r="AM3" s="13">
         <v>1</v>
       </c>
-      <c r="AN3" s="21">
+      <c r="AN3" s="13">
         <v>0.26</v>
       </c>
     </row>
@@ -1576,103 +1613,103 @@
       <c r="G4">
         <v>45</v>
       </c>
-      <c r="H4" s="24">
+      <c r="H4" s="15">
         <v>0.59699999999999998</v>
       </c>
-      <c r="I4" s="29">
+      <c r="I4" s="19">
         <v>1</v>
       </c>
-      <c r="J4" s="29">
+      <c r="J4" s="19">
         <v>0.33</v>
       </c>
-      <c r="K4" s="29" t="s">
+      <c r="K4" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="L4" s="29">
+      <c r="L4" s="19">
         <v>100</v>
       </c>
-      <c r="M4" s="32">
+      <c r="M4" s="21">
         <v>1</v>
       </c>
-      <c r="N4" s="32">
+      <c r="N4" s="21">
         <v>0.33</v>
       </c>
-      <c r="O4" s="32" t="s">
+      <c r="O4" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="P4" s="32">
+      <c r="P4" s="21">
         <v>100</v>
       </c>
-      <c r="Q4" s="21">
+      <c r="Q4" s="13">
         <v>0.79</v>
       </c>
-      <c r="R4" s="21">
+      <c r="R4" s="13">
         <v>0.16</v>
       </c>
-      <c r="S4" s="21">
+      <c r="S4" s="13">
         <v>0.79</v>
       </c>
-      <c r="T4" s="21">
+      <c r="T4" s="13">
         <v>0.16</v>
       </c>
-      <c r="U4" s="21">
+      <c r="U4" s="13">
         <v>0.79</v>
       </c>
-      <c r="V4" s="21">
+      <c r="V4" s="13">
         <v>0.16</v>
       </c>
-      <c r="W4" s="21">
+      <c r="W4" s="13">
         <v>0.62</v>
       </c>
-      <c r="X4" s="21">
+      <c r="X4" s="13">
         <v>0</v>
       </c>
-      <c r="Y4" s="21">
+      <c r="Y4" s="13">
         <v>0.62</v>
       </c>
-      <c r="Z4" s="21">
+      <c r="Z4" s="13">
         <v>0</v>
       </c>
-      <c r="AA4" s="21">
+      <c r="AA4" s="13">
         <v>0.62</v>
       </c>
-      <c r="AB4" s="21">
+      <c r="AB4" s="13">
         <v>0</v>
       </c>
-      <c r="AC4" s="21">
+      <c r="AC4" s="13">
         <v>0.64</v>
       </c>
-      <c r="AD4" s="21">
+      <c r="AD4" s="13">
         <v>0.06</v>
       </c>
-      <c r="AE4" s="21">
+      <c r="AE4" s="13">
         <v>0.65</v>
       </c>
-      <c r="AF4" s="21">
+      <c r="AF4" s="13">
         <v>0.05</v>
       </c>
-      <c r="AG4" s="21">
+      <c r="AG4" s="13">
         <v>0.8</v>
       </c>
-      <c r="AH4" s="21">
+      <c r="AH4" s="13">
         <v>0.22</v>
       </c>
-      <c r="AI4" s="21">
+      <c r="AI4" s="13">
         <v>0.71</v>
       </c>
-      <c r="AJ4" s="21">
+      <c r="AJ4" s="13">
         <v>0.13</v>
       </c>
-      <c r="AK4" s="21">
+      <c r="AK4" s="13">
         <v>0.69</v>
       </c>
-      <c r="AL4" s="21">
+      <c r="AL4" s="13">
         <v>0.12</v>
       </c>
-      <c r="AM4" s="21">
+      <c r="AM4" s="13">
         <v>1</v>
       </c>
-      <c r="AN4" s="21">
+      <c r="AN4" s="13">
         <v>0.33</v>
       </c>
     </row>
@@ -1698,103 +1735,103 @@
       <c r="G5">
         <v>37</v>
       </c>
-      <c r="H5" s="24">
+      <c r="H5" s="15">
         <v>0.45600000000000002</v>
       </c>
-      <c r="I5" s="29">
+      <c r="I5" s="19">
         <v>1</v>
       </c>
-      <c r="J5" s="29">
+      <c r="J5" s="19">
         <v>0.5</v>
       </c>
-      <c r="K5" s="29" t="s">
+      <c r="K5" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="L5" s="29">
+      <c r="L5" s="19">
         <v>100</v>
       </c>
-      <c r="M5" s="32">
+      <c r="M5" s="21">
         <v>1</v>
       </c>
-      <c r="N5" s="32">
+      <c r="N5" s="21">
         <v>0.5</v>
       </c>
-      <c r="O5" s="32" t="s">
+      <c r="O5" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="P5" s="32">
+      <c r="P5" s="21">
         <v>100</v>
       </c>
-      <c r="Q5" s="21">
+      <c r="Q5" s="13">
         <v>0.61</v>
       </c>
-      <c r="R5" s="21">
+      <c r="R5" s="13">
         <v>0.19</v>
       </c>
-      <c r="S5" s="21">
+      <c r="S5" s="13">
         <v>0.6</v>
       </c>
-      <c r="T5" s="21">
+      <c r="T5" s="13">
         <v>0.18</v>
       </c>
-      <c r="U5" s="21">
+      <c r="U5" s="13">
         <v>0.61</v>
       </c>
-      <c r="V5" s="21">
+      <c r="V5" s="13">
         <v>0.19</v>
       </c>
-      <c r="W5" s="21">
+      <c r="W5" s="13">
         <v>0.49</v>
       </c>
-      <c r="X5" s="21">
+      <c r="X5" s="13">
         <v>0.01</v>
       </c>
-      <c r="Y5" s="21">
+      <c r="Y5" s="13">
         <v>0.49</v>
       </c>
-      <c r="Z5" s="21">
+      <c r="Z5" s="13">
         <v>0.01</v>
       </c>
-      <c r="AA5" s="21">
+      <c r="AA5" s="13">
         <v>0.49</v>
       </c>
-      <c r="AB5" s="21">
+      <c r="AB5" s="13">
         <v>0.01</v>
       </c>
-      <c r="AC5" s="21">
+      <c r="AC5" s="13">
         <v>0.59</v>
       </c>
-      <c r="AD5" s="21">
+      <c r="AD5" s="13">
         <v>0.12</v>
       </c>
-      <c r="AE5" s="21">
+      <c r="AE5" s="13">
         <v>0.61</v>
       </c>
-      <c r="AF5" s="21">
+      <c r="AF5" s="13">
         <v>0.11</v>
       </c>
-      <c r="AG5" s="21">
+      <c r="AG5" s="13">
         <v>0.79</v>
       </c>
-      <c r="AH5" s="21">
+      <c r="AH5" s="13">
         <v>0.33</v>
       </c>
-      <c r="AI5" s="21">
+      <c r="AI5" s="13">
         <v>0.69</v>
       </c>
-      <c r="AJ5" s="21">
+      <c r="AJ5" s="13">
         <v>0.23</v>
       </c>
-      <c r="AK5" s="21">
+      <c r="AK5" s="13">
         <v>0.65</v>
       </c>
-      <c r="AL5" s="21">
+      <c r="AL5" s="13">
         <v>0.2</v>
       </c>
-      <c r="AM5" s="21">
+      <c r="AM5" s="13">
         <v>1</v>
       </c>
-      <c r="AN5" s="21">
+      <c r="AN5" s="13">
         <v>0.5</v>
       </c>
     </row>
@@ -1820,103 +1857,103 @@
       <c r="G6">
         <v>29</v>
       </c>
-      <c r="H6" s="24">
+      <c r="H6" s="15">
         <v>0.40300000000000002</v>
       </c>
-      <c r="I6" s="29">
+      <c r="I6" s="19">
         <v>1</v>
       </c>
-      <c r="J6" s="29">
+      <c r="J6" s="19">
         <v>0.46</v>
       </c>
-      <c r="K6" s="29" t="s">
+      <c r="K6" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="L6" s="29">
+      <c r="L6" s="19">
         <v>100</v>
       </c>
-      <c r="M6" s="32">
+      <c r="M6" s="21">
         <v>1</v>
       </c>
-      <c r="N6" s="32">
+      <c r="N6" s="21">
         <v>0.46</v>
       </c>
-      <c r="O6" s="32" t="s">
+      <c r="O6" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="P6" s="32">
+      <c r="P6" s="21">
         <v>100</v>
       </c>
-      <c r="Q6" s="21">
+      <c r="Q6" s="13">
         <v>0.64</v>
       </c>
-      <c r="R6" s="21">
+      <c r="R6" s="13">
         <v>0.17</v>
       </c>
-      <c r="S6" s="21">
+      <c r="S6" s="13">
         <v>0.64</v>
       </c>
-      <c r="T6" s="21">
+      <c r="T6" s="13">
         <v>0.17</v>
       </c>
-      <c r="U6" s="21">
+      <c r="U6" s="13">
         <v>0.64</v>
       </c>
-      <c r="V6" s="21">
+      <c r="V6" s="13">
         <v>0.17</v>
       </c>
-      <c r="W6" s="21">
+      <c r="W6" s="13">
         <v>0.43</v>
       </c>
-      <c r="X6" s="21">
+      <c r="X6" s="13">
         <v>0.01</v>
       </c>
-      <c r="Y6" s="21">
+      <c r="Y6" s="13">
         <v>0.43</v>
       </c>
-      <c r="Z6" s="21">
+      <c r="Z6" s="13">
         <v>0.01</v>
       </c>
-      <c r="AA6" s="21">
+      <c r="AA6" s="13">
         <v>0.43</v>
       </c>
-      <c r="AB6" s="21">
+      <c r="AB6" s="13">
         <v>0.01</v>
       </c>
-      <c r="AC6" s="21">
+      <c r="AC6" s="13">
         <v>0.46</v>
       </c>
-      <c r="AD6" s="21">
+      <c r="AD6" s="13">
         <v>0.1</v>
       </c>
-      <c r="AE6" s="21">
+      <c r="AE6" s="13">
         <v>0.52</v>
       </c>
-      <c r="AF6" s="21">
+      <c r="AF6" s="13">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AG6" s="21">
+      <c r="AG6" s="13">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AH6" s="21">
+      <c r="AH6" s="13">
         <v>0.28000000000000003</v>
       </c>
-      <c r="AI6" s="21">
+      <c r="AI6" s="13">
         <v>0.69</v>
       </c>
-      <c r="AJ6" s="21">
+      <c r="AJ6" s="13">
         <v>0.23</v>
       </c>
-      <c r="AK6" s="21">
+      <c r="AK6" s="13">
         <v>0.65</v>
       </c>
-      <c r="AL6" s="21">
+      <c r="AL6" s="13">
         <v>0.2</v>
       </c>
-      <c r="AM6" s="21">
+      <c r="AM6" s="13">
         <v>1</v>
       </c>
-      <c r="AN6" s="21">
+      <c r="AN6" s="13">
         <v>0.46</v>
       </c>
     </row>
@@ -1942,103 +1979,103 @@
       <c r="G7">
         <v>4392</v>
       </c>
-      <c r="H7" s="24">
+      <c r="H7" s="15">
         <v>0.46</v>
       </c>
-      <c r="I7" s="29">
+      <c r="I7" s="19">
         <v>1</v>
       </c>
-      <c r="J7" s="29">
+      <c r="J7" s="19">
         <v>0.23</v>
       </c>
-      <c r="K7" s="29" t="s">
+      <c r="K7" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="L7" s="29">
+      <c r="L7" s="19">
         <v>100</v>
       </c>
-      <c r="M7" s="32">
+      <c r="M7" s="21">
         <v>1</v>
       </c>
-      <c r="N7" s="32">
+      <c r="N7" s="21">
         <v>0.23</v>
       </c>
-      <c r="O7" s="32" t="s">
+      <c r="O7" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="P7" s="32">
+      <c r="P7" s="21">
         <v>100</v>
       </c>
-      <c r="Q7" s="21">
+      <c r="Q7" s="13">
         <v>0.62</v>
       </c>
-      <c r="R7" s="21">
+      <c r="R7" s="13">
         <v>0.03</v>
       </c>
-      <c r="S7" s="21">
+      <c r="S7" s="13">
         <v>0.62</v>
       </c>
-      <c r="T7" s="21">
+      <c r="T7" s="13">
         <v>0.03</v>
       </c>
-      <c r="U7" s="21">
+      <c r="U7" s="13">
         <v>0.62</v>
       </c>
-      <c r="V7" s="21">
+      <c r="V7" s="13">
         <v>0.03</v>
       </c>
-      <c r="W7" s="21">
+      <c r="W7" s="13">
         <v>0.43</v>
       </c>
-      <c r="X7" s="21">
+      <c r="X7" s="13">
         <v>0</v>
       </c>
-      <c r="Y7" s="21">
+      <c r="Y7" s="13">
         <v>0.43</v>
       </c>
-      <c r="Z7" s="21">
+      <c r="Z7" s="13">
         <v>0</v>
       </c>
-      <c r="AA7" s="21">
+      <c r="AA7" s="13">
         <v>0.43</v>
       </c>
-      <c r="AB7" s="21">
+      <c r="AB7" s="13">
         <v>0</v>
       </c>
-      <c r="AC7" s="21">
+      <c r="AC7" s="13">
         <v>0.54</v>
       </c>
-      <c r="AD7" s="21">
+      <c r="AD7" s="13">
         <v>0.04</v>
       </c>
-      <c r="AE7" s="21">
+      <c r="AE7" s="13">
         <v>0.55000000000000004</v>
       </c>
-      <c r="AF7" s="21">
+      <c r="AF7" s="13">
         <v>0.02</v>
       </c>
-      <c r="AG7" s="21">
+      <c r="AG7" s="13">
         <v>0.59</v>
       </c>
-      <c r="AH7" s="21">
+      <c r="AH7" s="13">
         <v>0.16</v>
       </c>
-      <c r="AI7" s="21">
+      <c r="AI7" s="13">
         <v>0.77</v>
       </c>
-      <c r="AJ7" s="21">
+      <c r="AJ7" s="13">
         <v>0.06</v>
       </c>
-      <c r="AK7" s="21">
+      <c r="AK7" s="13">
         <v>0.73</v>
       </c>
-      <c r="AL7" s="21">
+      <c r="AL7" s="13">
         <v>0.03</v>
       </c>
-      <c r="AM7" s="21">
+      <c r="AM7" s="13">
         <v>1</v>
       </c>
-      <c r="AN7" s="21">
+      <c r="AN7" s="13">
         <v>0.23</v>
       </c>
     </row>
@@ -2064,103 +2101,103 @@
       <c r="G8">
         <v>1422</v>
       </c>
-      <c r="H8" s="24">
+      <c r="H8" s="15">
         <v>0.219</v>
       </c>
-      <c r="I8" s="29">
+      <c r="I8" s="19">
         <v>1</v>
       </c>
-      <c r="J8" s="29">
+      <c r="J8" s="19">
         <v>0.47</v>
       </c>
-      <c r="K8" s="29" t="s">
+      <c r="K8" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="L8" s="29">
+      <c r="L8" s="19">
         <v>100</v>
       </c>
-      <c r="M8" s="32">
+      <c r="M8" s="21">
         <v>1</v>
       </c>
-      <c r="N8" s="32">
+      <c r="N8" s="21">
         <v>0.47</v>
       </c>
-      <c r="O8" s="32" t="s">
+      <c r="O8" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="P8" s="32">
+      <c r="P8" s="21">
         <v>100</v>
       </c>
-      <c r="Q8" s="21">
+      <c r="Q8" s="13">
         <v>0.33</v>
       </c>
-      <c r="R8" s="21">
+      <c r="R8" s="13">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="S8" s="21">
+      <c r="S8" s="13">
         <v>0.33</v>
       </c>
-      <c r="T8" s="21">
+      <c r="T8" s="13">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="U8" s="21">
+      <c r="U8" s="13">
         <v>0.33</v>
       </c>
-      <c r="V8" s="21">
+      <c r="V8" s="13">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="W8" s="21">
+      <c r="W8" s="13">
         <v>0.19</v>
       </c>
-      <c r="X8" s="21">
+      <c r="X8" s="13">
         <v>0</v>
       </c>
-      <c r="Y8" s="21">
+      <c r="Y8" s="13">
         <v>0.19</v>
       </c>
-      <c r="Z8" s="21">
+      <c r="Z8" s="13">
         <v>0</v>
       </c>
-      <c r="AA8" s="21">
+      <c r="AA8" s="13">
         <v>0.19</v>
       </c>
-      <c r="AB8" s="21">
+      <c r="AB8" s="13">
         <v>0</v>
       </c>
-      <c r="AC8" s="21">
+      <c r="AC8" s="13">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AD8" s="21">
+      <c r="AD8" s="13">
         <v>0.1</v>
       </c>
-      <c r="AE8" s="21">
+      <c r="AE8" s="13">
         <v>0.28000000000000003</v>
       </c>
-      <c r="AF8" s="21">
+      <c r="AF8" s="13">
         <v>0.03</v>
       </c>
-      <c r="AG8" s="21">
+      <c r="AG8" s="13">
         <v>0.28000000000000003</v>
       </c>
-      <c r="AH8" s="21">
+      <c r="AH8" s="13">
         <v>0.37</v>
       </c>
-      <c r="AI8" s="21">
+      <c r="AI8" s="13">
         <v>0.49</v>
       </c>
-      <c r="AJ8" s="21">
+      <c r="AJ8" s="13">
         <v>0.11</v>
       </c>
-      <c r="AK8" s="21">
+      <c r="AK8" s="13">
         <v>0.42</v>
       </c>
-      <c r="AL8" s="21">
+      <c r="AL8" s="13">
         <v>0.05</v>
       </c>
-      <c r="AM8" s="21">
+      <c r="AM8" s="13">
         <v>1</v>
       </c>
-      <c r="AN8" s="21">
+      <c r="AN8" s="13">
         <v>0.47</v>
       </c>
     </row>
@@ -2186,103 +2223,103 @@
       <c r="G9">
         <v>786</v>
       </c>
-      <c r="H9" s="24">
+      <c r="H9" s="15">
         <v>0.151</v>
       </c>
-      <c r="I9" s="29">
+      <c r="I9" s="19">
         <v>1</v>
       </c>
-      <c r="J9" s="29">
+      <c r="J9" s="19">
         <v>0.62</v>
       </c>
-      <c r="K9" s="29" t="s">
+      <c r="K9" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="L9" s="29">
+      <c r="L9" s="19">
         <v>100</v>
       </c>
-      <c r="M9" s="32">
+      <c r="M9" s="21">
         <v>1</v>
       </c>
-      <c r="N9" s="32">
+      <c r="N9" s="21">
         <v>0.62</v>
       </c>
-      <c r="O9" s="32" t="s">
+      <c r="O9" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="P9" s="32">
+      <c r="P9" s="21">
         <v>100</v>
       </c>
-      <c r="Q9" s="21">
+      <c r="Q9" s="13">
         <v>0.21</v>
       </c>
-      <c r="R9" s="21">
+      <c r="R9" s="13">
         <v>0.08</v>
       </c>
-      <c r="S9" s="21">
+      <c r="S9" s="13">
         <v>0.22</v>
       </c>
-      <c r="T9" s="21">
+      <c r="T9" s="13">
         <v>0.08</v>
       </c>
-      <c r="U9" s="21">
+      <c r="U9" s="13">
         <v>0.21</v>
       </c>
-      <c r="V9" s="21">
+      <c r="V9" s="13">
         <v>0.08</v>
       </c>
-      <c r="W9" s="21">
+      <c r="W9" s="13">
         <v>0.13</v>
       </c>
-      <c r="X9" s="21">
+      <c r="X9" s="13">
         <v>0</v>
       </c>
-      <c r="Y9" s="21">
+      <c r="Y9" s="13">
         <v>0.13</v>
       </c>
-      <c r="Z9" s="21">
+      <c r="Z9" s="13">
         <v>0</v>
       </c>
-      <c r="AA9" s="21">
+      <c r="AA9" s="13">
         <v>0.13</v>
       </c>
-      <c r="AB9" s="21">
+      <c r="AB9" s="13">
         <v>0</v>
       </c>
-      <c r="AC9" s="21">
+      <c r="AC9" s="13">
         <v>0.19</v>
       </c>
-      <c r="AD9" s="21">
+      <c r="AD9" s="13">
         <v>0.12</v>
       </c>
-      <c r="AE9" s="21">
+      <c r="AE9" s="13">
         <v>0.18</v>
       </c>
-      <c r="AF9" s="21">
+      <c r="AF9" s="13">
         <v>0.02</v>
       </c>
-      <c r="AG9" s="21">
+      <c r="AG9" s="13">
         <v>0.14000000000000001</v>
       </c>
-      <c r="AH9" s="21">
+      <c r="AH9" s="13">
         <v>0.45</v>
       </c>
-      <c r="AI9" s="21">
+      <c r="AI9" s="13">
         <v>0.33</v>
       </c>
-      <c r="AJ9" s="21">
+      <c r="AJ9" s="13">
         <v>0.12</v>
       </c>
-      <c r="AK9" s="21">
+      <c r="AK9" s="13">
         <v>0.3</v>
       </c>
-      <c r="AL9" s="21">
+      <c r="AL9" s="13">
         <v>0.04</v>
       </c>
-      <c r="AM9" s="21">
+      <c r="AM9" s="13">
         <v>1</v>
       </c>
-      <c r="AN9" s="21">
+      <c r="AN9" s="13">
         <v>0.62</v>
       </c>
     </row>
@@ -2308,103 +2345,103 @@
       <c r="G10">
         <v>611</v>
       </c>
-      <c r="H10" s="24">
+      <c r="H10" s="15">
         <v>0.124</v>
       </c>
-      <c r="I10" s="29">
+      <c r="I10" s="19">
         <v>1</v>
       </c>
-      <c r="J10" s="29">
+      <c r="J10" s="19">
         <v>0.72</v>
       </c>
-      <c r="K10" s="29" t="s">
+      <c r="K10" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="L10" s="29">
+      <c r="L10" s="19">
         <v>100</v>
       </c>
-      <c r="M10" s="32">
+      <c r="M10" s="21">
         <v>1</v>
       </c>
-      <c r="N10" s="32">
+      <c r="N10" s="21">
         <v>0.72</v>
       </c>
-      <c r="O10" s="32" t="s">
+      <c r="O10" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="P10" s="32">
+      <c r="P10" s="21">
         <v>100</v>
       </c>
-      <c r="Q10" s="21">
+      <c r="Q10" s="13">
         <v>0.16</v>
       </c>
-      <c r="R10" s="21">
+      <c r="R10" s="13">
         <v>0.13</v>
       </c>
-      <c r="S10" s="21">
+      <c r="S10" s="13">
         <v>0.16</v>
       </c>
-      <c r="T10" s="21">
+      <c r="T10" s="13">
         <v>0.13</v>
       </c>
-      <c r="U10" s="21">
+      <c r="U10" s="13">
         <v>0.16</v>
       </c>
-      <c r="V10" s="21">
+      <c r="V10" s="13">
         <v>0.13</v>
       </c>
-      <c r="W10" s="21">
+      <c r="W10" s="13">
         <v>0.1</v>
       </c>
-      <c r="X10" s="21">
+      <c r="X10" s="13">
         <v>0</v>
       </c>
-      <c r="Y10" s="21">
+      <c r="Y10" s="13">
         <v>0.1</v>
       </c>
-      <c r="Z10" s="21">
+      <c r="Z10" s="13">
         <v>0</v>
       </c>
-      <c r="AA10" s="21">
+      <c r="AA10" s="13">
         <v>0.1</v>
       </c>
-      <c r="AB10" s="21">
+      <c r="AB10" s="13">
         <v>0</v>
       </c>
-      <c r="AC10" s="21">
+      <c r="AC10" s="13">
         <v>0.15</v>
       </c>
-      <c r="AD10" s="21">
+      <c r="AD10" s="13">
         <v>0.16</v>
       </c>
-      <c r="AE10" s="21">
+      <c r="AE10" s="13">
         <v>0.16</v>
       </c>
-      <c r="AF10" s="21">
+      <c r="AF10" s="13">
         <v>0.02</v>
       </c>
-      <c r="AG10" s="21">
+      <c r="AG10" s="13">
         <v>0.08</v>
       </c>
-      <c r="AH10" s="21">
+      <c r="AH10" s="13">
         <v>0.54</v>
       </c>
-      <c r="AI10" s="21">
+      <c r="AI10" s="13">
         <v>0.26</v>
       </c>
-      <c r="AJ10" s="21">
+      <c r="AJ10" s="13">
         <v>0.17</v>
       </c>
-      <c r="AK10" s="21">
+      <c r="AK10" s="13">
         <v>0.23</v>
       </c>
-      <c r="AL10" s="21">
+      <c r="AL10" s="13">
         <v>0.04</v>
       </c>
-      <c r="AM10" s="21">
+      <c r="AM10" s="13">
         <v>1</v>
       </c>
-      <c r="AN10" s="21">
+      <c r="AN10" s="13">
         <v>0.72</v>
       </c>
     </row>
@@ -2424,109 +2461,109 @@
       <c r="E11">
         <v>0.01</v>
       </c>
-      <c r="F11" s="20">
+      <c r="F11" s="12">
         <v>14</v>
       </c>
       <c r="G11">
         <v>700</v>
       </c>
-      <c r="H11" s="24">
+      <c r="H11" s="15">
         <v>0.49399999999999999</v>
       </c>
-      <c r="I11" s="29">
+      <c r="I11" s="19">
         <v>0.52</v>
       </c>
-      <c r="J11" s="29">
+      <c r="J11" s="19">
         <v>0.37</v>
       </c>
-      <c r="K11" s="29" t="s">
+      <c r="K11" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="L11" s="29">
+      <c r="L11" s="19">
         <v>100</v>
       </c>
-      <c r="M11" s="32">
+      <c r="M11" s="21">
         <v>0.48</v>
       </c>
-      <c r="N11" s="32">
+      <c r="N11" s="21">
         <v>0.24</v>
       </c>
-      <c r="O11" s="32" t="s">
+      <c r="O11" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="P11" s="32">
+      <c r="P11" s="21">
         <v>50</v>
       </c>
-      <c r="Q11" s="21">
+      <c r="Q11" s="13">
         <v>0.5</v>
       </c>
-      <c r="R11" s="21">
+      <c r="R11" s="13">
         <v>0.27</v>
       </c>
-      <c r="S11" s="21">
+      <c r="S11" s="13">
         <v>0.5</v>
       </c>
-      <c r="T11" s="21">
+      <c r="T11" s="13">
         <v>0.27</v>
       </c>
-      <c r="U11" s="21">
+      <c r="U11" s="13">
         <v>0.5</v>
       </c>
-      <c r="V11" s="21">
+      <c r="V11" s="13">
         <v>0.27</v>
       </c>
-      <c r="W11" s="21">
+      <c r="W11" s="13">
         <v>0.48</v>
       </c>
-      <c r="X11" s="21">
+      <c r="X11" s="13">
         <v>0.24</v>
       </c>
-      <c r="Y11" s="21">
+      <c r="Y11" s="13">
         <v>0.48</v>
       </c>
-      <c r="Z11" s="21">
+      <c r="Z11" s="13">
         <v>0.24</v>
       </c>
-      <c r="AA11" s="21">
+      <c r="AA11" s="13">
         <v>0.48</v>
       </c>
-      <c r="AB11" s="21">
+      <c r="AB11" s="13">
         <v>0.24</v>
       </c>
-      <c r="AC11" s="21">
+      <c r="AC11" s="13">
         <v>0.49</v>
       </c>
-      <c r="AD11" s="21">
+      <c r="AD11" s="13">
         <v>0.3</v>
       </c>
-      <c r="AE11" s="21">
+      <c r="AE11" s="13">
         <v>0.49</v>
       </c>
-      <c r="AF11" s="21">
+      <c r="AF11" s="13">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AG11" s="21">
+      <c r="AG11" s="13">
         <v>0.5</v>
       </c>
-      <c r="AH11" s="21">
+      <c r="AH11" s="13">
         <v>0.34</v>
       </c>
-      <c r="AI11" s="21">
+      <c r="AI11" s="13">
         <v>0.5</v>
       </c>
-      <c r="AJ11" s="21">
+      <c r="AJ11" s="13">
         <v>0.31</v>
       </c>
-      <c r="AK11" s="21">
+      <c r="AK11" s="13">
         <v>0.5</v>
       </c>
-      <c r="AL11" s="21">
+      <c r="AL11" s="13">
         <v>0.3</v>
       </c>
-      <c r="AM11" s="21">
+      <c r="AM11" s="13">
         <v>0.52</v>
       </c>
-      <c r="AN11" s="21">
+      <c r="AN11" s="13">
         <v>0.37</v>
       </c>
     </row>
@@ -2546,109 +2583,109 @@
       <c r="E12">
         <v>0.02</v>
       </c>
-      <c r="F12" s="20">
+      <c r="F12" s="12">
         <v>15</v>
       </c>
       <c r="G12">
         <v>700</v>
       </c>
-      <c r="H12" s="24">
+      <c r="H12" s="15">
         <v>0.33</v>
       </c>
-      <c r="I12" s="29">
+      <c r="I12" s="19">
         <v>0.39</v>
       </c>
-      <c r="J12" s="29">
+      <c r="J12" s="19">
         <v>0.4</v>
       </c>
-      <c r="K12" s="29" t="s">
+      <c r="K12" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="L12" s="29">
+      <c r="L12" s="19">
         <v>100</v>
       </c>
-      <c r="M12" s="32">
+      <c r="M12" s="21">
         <v>0.31</v>
       </c>
-      <c r="N12" s="32">
+      <c r="N12" s="21">
         <v>0.13</v>
       </c>
-      <c r="O12" s="32" t="s">
+      <c r="O12" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="P12" s="32">
+      <c r="P12" s="21">
         <v>50</v>
       </c>
-      <c r="Q12" s="21">
+      <c r="Q12" s="13">
         <v>0.31</v>
       </c>
-      <c r="R12" s="21">
+      <c r="R12" s="13">
         <v>0.2</v>
       </c>
-      <c r="S12" s="21">
+      <c r="S12" s="13">
         <v>0.31</v>
       </c>
-      <c r="T12" s="21">
+      <c r="T12" s="13">
         <v>0.2</v>
       </c>
-      <c r="U12" s="21">
+      <c r="U12" s="13">
         <v>0.31</v>
       </c>
-      <c r="V12" s="21">
+      <c r="V12" s="13">
         <v>0.2</v>
       </c>
-      <c r="W12" s="21">
+      <c r="W12" s="13">
         <v>0.31</v>
       </c>
-      <c r="X12" s="21">
+      <c r="X12" s="13">
         <v>0.13</v>
       </c>
-      <c r="Y12" s="21">
+      <c r="Y12" s="13">
         <v>0.31</v>
       </c>
-      <c r="Z12" s="21">
+      <c r="Z12" s="13">
         <v>0.13</v>
       </c>
-      <c r="AA12" s="21">
+      <c r="AA12" s="13">
         <v>0.31</v>
       </c>
-      <c r="AB12" s="21">
+      <c r="AB12" s="13">
         <v>0.13</v>
       </c>
-      <c r="AC12" s="21">
+      <c r="AC12" s="13">
         <v>0.33</v>
       </c>
-      <c r="AD12" s="21">
+      <c r="AD12" s="13">
         <v>0.25</v>
       </c>
-      <c r="AE12" s="21">
+      <c r="AE12" s="13">
         <v>0.33</v>
       </c>
-      <c r="AF12" s="21">
+      <c r="AF12" s="13">
         <v>0.22</v>
       </c>
-      <c r="AG12" s="21">
+      <c r="AG12" s="13">
         <v>0.37</v>
       </c>
-      <c r="AH12" s="21">
+      <c r="AH12" s="13">
         <v>0.35</v>
       </c>
-      <c r="AI12" s="21">
+      <c r="AI12" s="13">
         <v>0.33</v>
       </c>
-      <c r="AJ12" s="21">
+      <c r="AJ12" s="13">
         <v>0.28000000000000003</v>
       </c>
-      <c r="AK12" s="21">
+      <c r="AK12" s="13">
         <v>0.35</v>
       </c>
-      <c r="AL12" s="21">
+      <c r="AL12" s="13">
         <v>0.25</v>
       </c>
-      <c r="AM12" s="21">
+      <c r="AM12" s="13">
         <v>0.39</v>
       </c>
-      <c r="AN12" s="21">
+      <c r="AN12" s="13">
         <v>0.4</v>
       </c>
     </row>
@@ -2668,109 +2705,109 @@
       <c r="E13">
         <v>0.03</v>
       </c>
-      <c r="F13" s="20">
+      <c r="F13" s="12">
         <v>19</v>
       </c>
       <c r="G13">
         <v>700</v>
       </c>
-      <c r="H13" s="24">
+      <c r="H13" s="15">
         <v>0.28399999999999997</v>
       </c>
-      <c r="I13" s="29">
+      <c r="I13" s="19">
         <v>0.36</v>
       </c>
-      <c r="J13" s="29">
+      <c r="J13" s="19">
         <v>0.44</v>
       </c>
-      <c r="K13" s="29" t="s">
+      <c r="K13" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="L13" s="29">
+      <c r="L13" s="19">
         <v>100</v>
       </c>
-      <c r="M13" s="32">
+      <c r="M13" s="21">
         <v>0.28000000000000003</v>
       </c>
-      <c r="N13" s="32">
+      <c r="N13" s="21">
         <v>0.06</v>
       </c>
-      <c r="O13" s="32" t="s">
+      <c r="O13" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="P13" s="32">
+      <c r="P13" s="21">
         <v>50</v>
       </c>
-      <c r="Q13" s="21">
+      <c r="Q13" s="13">
         <v>0.28000000000000003</v>
       </c>
-      <c r="R13" s="21">
+      <c r="R13" s="13">
         <v>0.15</v>
       </c>
-      <c r="S13" s="21">
+      <c r="S13" s="13">
         <v>0.28000000000000003</v>
       </c>
-      <c r="T13" s="21">
+      <c r="T13" s="13">
         <v>0.15</v>
       </c>
-      <c r="U13" s="21">
+      <c r="U13" s="13">
         <v>0.28000000000000003</v>
       </c>
-      <c r="V13" s="21">
+      <c r="V13" s="13">
         <v>0.15</v>
       </c>
-      <c r="W13" s="21">
+      <c r="W13" s="13">
         <v>0.28000000000000003</v>
       </c>
-      <c r="X13" s="21">
+      <c r="X13" s="13">
         <v>0.06</v>
       </c>
-      <c r="Y13" s="21">
+      <c r="Y13" s="13">
         <v>0.28000000000000003</v>
       </c>
-      <c r="Z13" s="21">
+      <c r="Z13" s="13">
         <v>0.06</v>
       </c>
-      <c r="AA13" s="21">
+      <c r="AA13" s="13">
         <v>0.28000000000000003</v>
       </c>
-      <c r="AB13" s="21">
+      <c r="AB13" s="13">
         <v>0.06</v>
       </c>
-      <c r="AC13" s="21">
+      <c r="AC13" s="13">
         <v>0.27</v>
       </c>
-      <c r="AD13" s="21">
+      <c r="AD13" s="13">
         <v>0.2</v>
       </c>
-      <c r="AE13" s="21">
+      <c r="AE13" s="13">
         <v>0.27</v>
       </c>
-      <c r="AF13" s="21">
+      <c r="AF13" s="13">
         <v>0.14000000000000001</v>
       </c>
-      <c r="AG13" s="21">
+      <c r="AG13" s="13">
         <v>0.33</v>
       </c>
-      <c r="AH13" s="21">
+      <c r="AH13" s="13">
         <v>0.38</v>
       </c>
-      <c r="AI13" s="21">
+      <c r="AI13" s="13">
         <v>0.27</v>
       </c>
-      <c r="AJ13" s="21">
+      <c r="AJ13" s="13">
         <v>0.23</v>
       </c>
-      <c r="AK13" s="21">
+      <c r="AK13" s="13">
         <v>0.28000000000000003</v>
       </c>
-      <c r="AL13" s="21">
+      <c r="AL13" s="13">
         <v>0.16</v>
       </c>
-      <c r="AM13" s="21">
+      <c r="AM13" s="13">
         <v>0.36</v>
       </c>
-      <c r="AN13" s="21">
+      <c r="AN13" s="13">
         <v>0.44</v>
       </c>
     </row>
@@ -2790,109 +2827,109 @@
       <c r="E14">
         <v>0.04</v>
       </c>
-      <c r="F14" s="20">
+      <c r="F14" s="12">
         <v>18</v>
       </c>
       <c r="G14">
         <v>700</v>
       </c>
-      <c r="H14" s="24">
+      <c r="H14" s="15">
         <v>0.247</v>
       </c>
-      <c r="I14" s="29">
+      <c r="I14" s="19">
         <v>0.41</v>
       </c>
-      <c r="J14" s="29">
+      <c r="J14" s="19">
         <v>0.5</v>
       </c>
-      <c r="K14" s="29" t="s">
+      <c r="K14" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="L14" s="29">
+      <c r="L14" s="19">
         <v>100</v>
       </c>
-      <c r="M14" s="32">
+      <c r="M14" s="21">
         <v>0.25</v>
       </c>
-      <c r="N14" s="32">
+      <c r="N14" s="21">
         <v>0.04</v>
       </c>
-      <c r="O14" s="32" t="s">
+      <c r="O14" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="P14" s="32">
+      <c r="P14" s="21">
         <v>50</v>
       </c>
-      <c r="Q14" s="21">
+      <c r="Q14" s="13">
         <v>0.26</v>
       </c>
-      <c r="R14" s="21">
+      <c r="R14" s="13">
         <v>0.11</v>
       </c>
-      <c r="S14" s="21">
+      <c r="S14" s="13">
         <v>0.27</v>
       </c>
-      <c r="T14" s="21">
+      <c r="T14" s="13">
         <v>0.11</v>
       </c>
-      <c r="U14" s="21">
+      <c r="U14" s="13">
         <v>0.26</v>
       </c>
-      <c r="V14" s="21">
+      <c r="V14" s="13">
         <v>0.11</v>
       </c>
-      <c r="W14" s="21">
+      <c r="W14" s="13">
         <v>0.25</v>
       </c>
-      <c r="X14" s="21">
+      <c r="X14" s="13">
         <v>0.04</v>
       </c>
-      <c r="Y14" s="21">
+      <c r="Y14" s="13">
         <v>0.25</v>
       </c>
-      <c r="Z14" s="21">
+      <c r="Z14" s="13">
         <v>0.04</v>
       </c>
-      <c r="AA14" s="21">
+      <c r="AA14" s="13">
         <v>0.25</v>
       </c>
-      <c r="AB14" s="21">
+      <c r="AB14" s="13">
         <v>0.04</v>
       </c>
-      <c r="AC14" s="21">
+      <c r="AC14" s="13">
         <v>0.24</v>
       </c>
-      <c r="AD14" s="21">
+      <c r="AD14" s="13">
         <v>0.18</v>
       </c>
-      <c r="AE14" s="21">
+      <c r="AE14" s="13">
         <v>0.26</v>
       </c>
-      <c r="AF14" s="21">
+      <c r="AF14" s="13">
         <v>0.12</v>
       </c>
-      <c r="AG14" s="21">
+      <c r="AG14" s="13">
         <v>0.4</v>
       </c>
-      <c r="AH14" s="21">
+      <c r="AH14" s="13">
         <v>0.45</v>
       </c>
-      <c r="AI14" s="21">
+      <c r="AI14" s="13">
         <v>0.24</v>
       </c>
-      <c r="AJ14" s="21">
+      <c r="AJ14" s="13">
         <v>0.21</v>
       </c>
-      <c r="AK14" s="21">
+      <c r="AK14" s="13">
         <v>0.27</v>
       </c>
-      <c r="AL14" s="21">
+      <c r="AL14" s="13">
         <v>0.14000000000000001</v>
       </c>
-      <c r="AM14" s="21">
+      <c r="AM14" s="13">
         <v>0.41</v>
       </c>
-      <c r="AN14" s="21">
+      <c r="AN14" s="13">
         <v>0.5</v>
       </c>
     </row>
@@ -2918,103 +2955,103 @@
       <c r="G15">
         <v>371</v>
       </c>
-      <c r="H15" s="24">
+      <c r="H15" s="15">
         <v>0.54300000000000004</v>
       </c>
-      <c r="I15" s="29">
+      <c r="I15" s="19">
         <v>1</v>
       </c>
-      <c r="J15" s="29">
+      <c r="J15" s="19">
         <v>0.67</v>
       </c>
-      <c r="K15" s="29" t="s">
+      <c r="K15" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="L15" s="29">
+      <c r="L15" s="19">
         <v>100</v>
       </c>
-      <c r="M15" s="32">
+      <c r="M15" s="21">
         <v>0.52</v>
       </c>
-      <c r="N15" s="32">
+      <c r="N15" s="21">
         <v>0</v>
       </c>
-      <c r="O15" s="32" t="s">
+      <c r="O15" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="P15" s="32">
+      <c r="P15" s="21">
         <v>50</v>
       </c>
-      <c r="Q15" s="21">
+      <c r="Q15" s="13">
         <v>0.55000000000000004</v>
       </c>
-      <c r="R15" s="21">
+      <c r="R15" s="13">
         <v>0.2</v>
       </c>
-      <c r="S15" s="21">
+      <c r="S15" s="13">
         <v>0.55000000000000004</v>
       </c>
-      <c r="T15" s="21">
+      <c r="T15" s="13">
         <v>0.2</v>
       </c>
-      <c r="U15" s="21">
+      <c r="U15" s="13">
         <v>0.55000000000000004</v>
       </c>
-      <c r="V15" s="21">
+      <c r="V15" s="13">
         <v>0.2</v>
       </c>
-      <c r="W15" s="21">
+      <c r="W15" s="13">
         <v>0.52</v>
       </c>
-      <c r="X15" s="21">
+      <c r="X15" s="13">
         <v>0</v>
       </c>
-      <c r="Y15" s="21">
+      <c r="Y15" s="13">
         <v>0.52</v>
       </c>
-      <c r="Z15" s="21">
+      <c r="Z15" s="13">
         <v>0</v>
       </c>
-      <c r="AA15" s="21">
+      <c r="AA15" s="13">
         <v>0.52</v>
       </c>
-      <c r="AB15" s="21">
+      <c r="AB15" s="13">
         <v>0</v>
       </c>
-      <c r="AC15" s="21">
+      <c r="AC15" s="13">
         <v>0.61</v>
       </c>
-      <c r="AD15" s="21">
+      <c r="AD15" s="13">
         <v>0.25</v>
       </c>
-      <c r="AE15" s="21">
+      <c r="AE15" s="13">
         <v>0.59</v>
       </c>
-      <c r="AF15" s="21">
+      <c r="AF15" s="13">
         <v>0.21</v>
       </c>
-      <c r="AG15" s="21">
+      <c r="AG15" s="13">
         <v>0.85</v>
       </c>
-      <c r="AH15" s="21">
+      <c r="AH15" s="13">
         <v>0.55000000000000004</v>
       </c>
-      <c r="AI15" s="21">
+      <c r="AI15" s="13">
         <v>0.59</v>
       </c>
-      <c r="AJ15" s="21">
+      <c r="AJ15" s="13">
         <v>0.28000000000000003</v>
       </c>
-      <c r="AK15" s="21">
+      <c r="AK15" s="13">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AL15" s="21">
+      <c r="AL15" s="13">
         <v>0.24</v>
       </c>
-      <c r="AM15" s="21">
+      <c r="AM15" s="13">
         <v>1</v>
       </c>
-      <c r="AN15" s="21">
+      <c r="AN15" s="13">
         <v>0.67</v>
       </c>
     </row>
@@ -3040,103 +3077,103 @@
       <c r="G16">
         <v>175</v>
       </c>
-      <c r="H16" s="24">
+      <c r="H16" s="15">
         <v>0.40400000000000003</v>
       </c>
-      <c r="I16" s="29">
+      <c r="I16" s="19">
         <v>1</v>
       </c>
-      <c r="J16" s="29">
+      <c r="J16" s="19">
         <v>0.8</v>
       </c>
-      <c r="K16" s="29" t="s">
+      <c r="K16" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="L16" s="29">
+      <c r="L16" s="19">
         <v>100</v>
       </c>
-      <c r="M16" s="32">
+      <c r="M16" s="21">
         <v>0.37</v>
       </c>
-      <c r="N16" s="32">
+      <c r="N16" s="21">
         <v>0</v>
       </c>
-      <c r="O16" s="32" t="s">
+      <c r="O16" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="P16" s="32">
+      <c r="P16" s="21">
         <v>50</v>
       </c>
-      <c r="Q16" s="21">
+      <c r="Q16" s="13">
         <v>0.38</v>
       </c>
-      <c r="R16" s="21">
+      <c r="R16" s="13">
         <v>0.22</v>
       </c>
-      <c r="S16" s="21">
+      <c r="S16" s="13">
         <v>0.38</v>
       </c>
-      <c r="T16" s="21">
+      <c r="T16" s="13">
         <v>0.22</v>
       </c>
-      <c r="U16" s="21">
+      <c r="U16" s="13">
         <v>0.38</v>
       </c>
-      <c r="V16" s="21">
+      <c r="V16" s="13">
         <v>0.22</v>
       </c>
-      <c r="W16" s="21">
+      <c r="W16" s="13">
         <v>0.37</v>
       </c>
-      <c r="X16" s="21">
+      <c r="X16" s="13">
         <v>0</v>
       </c>
-      <c r="Y16" s="21">
+      <c r="Y16" s="13">
         <v>0.37</v>
       </c>
-      <c r="Z16" s="21">
+      <c r="Z16" s="13">
         <v>0</v>
       </c>
-      <c r="AA16" s="21">
+      <c r="AA16" s="13">
         <v>0.37</v>
       </c>
-      <c r="AB16" s="21">
+      <c r="AB16" s="13">
         <v>0</v>
       </c>
-      <c r="AC16" s="21">
+      <c r="AC16" s="13">
         <v>0.45</v>
       </c>
-      <c r="AD16" s="21">
+      <c r="AD16" s="13">
         <v>0.33</v>
       </c>
-      <c r="AE16" s="21">
+      <c r="AE16" s="13">
         <v>0.41</v>
       </c>
-      <c r="AF16" s="21">
+      <c r="AF16" s="13">
         <v>0.21</v>
       </c>
-      <c r="AG16" s="21">
+      <c r="AG16" s="13">
         <v>0.73</v>
       </c>
-      <c r="AH16" s="21">
+      <c r="AH16" s="13">
         <v>0.69</v>
       </c>
-      <c r="AI16" s="21">
+      <c r="AI16" s="13">
         <v>0.44</v>
       </c>
-      <c r="AJ16" s="21">
+      <c r="AJ16" s="13">
         <v>0.34</v>
       </c>
-      <c r="AK16" s="21">
+      <c r="AK16" s="13">
         <v>0.38</v>
       </c>
-      <c r="AL16" s="21">
+      <c r="AL16" s="13">
         <v>0.25</v>
       </c>
-      <c r="AM16" s="21">
+      <c r="AM16" s="13">
         <v>1</v>
       </c>
-      <c r="AN16" s="21">
+      <c r="AN16" s="13">
         <v>0.8</v>
       </c>
     </row>
@@ -3162,103 +3199,103 @@
       <c r="G17">
         <v>119</v>
       </c>
-      <c r="H17" s="24">
+      <c r="H17" s="15">
         <v>0.39400000000000002</v>
       </c>
-      <c r="I17" s="29">
+      <c r="I17" s="19">
         <v>0.96</v>
       </c>
-      <c r="J17" s="29">
+      <c r="J17" s="19">
         <v>0.86</v>
       </c>
-      <c r="K17" s="29" t="s">
+      <c r="K17" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="L17" s="29">
+      <c r="L17" s="19">
         <v>100</v>
       </c>
-      <c r="M17" s="32">
+      <c r="M17" s="21">
         <v>0.37</v>
       </c>
-      <c r="N17" s="32">
+      <c r="N17" s="21">
         <v>0</v>
       </c>
-      <c r="O17" s="32" t="s">
+      <c r="O17" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="P17" s="32">
+      <c r="P17" s="21">
         <v>50</v>
       </c>
-      <c r="Q17" s="21">
+      <c r="Q17" s="13">
         <v>0.41</v>
       </c>
-      <c r="R17" s="21">
+      <c r="R17" s="13">
         <v>0.17</v>
       </c>
-      <c r="S17" s="21">
+      <c r="S17" s="13">
         <v>0.41</v>
       </c>
-      <c r="T17" s="21">
+      <c r="T17" s="13">
         <v>0.17</v>
       </c>
-      <c r="U17" s="21">
+      <c r="U17" s="13">
         <v>0.41</v>
       </c>
-      <c r="V17" s="21">
+      <c r="V17" s="13">
         <v>0.17</v>
       </c>
-      <c r="W17" s="21">
+      <c r="W17" s="13">
         <v>0.37</v>
       </c>
-      <c r="X17" s="21">
+      <c r="X17" s="13">
         <v>0</v>
       </c>
-      <c r="Y17" s="21">
+      <c r="Y17" s="13">
         <v>0.37</v>
       </c>
-      <c r="Z17" s="21">
+      <c r="Z17" s="13">
         <v>0</v>
       </c>
-      <c r="AA17" s="21">
+      <c r="AA17" s="13">
         <v>0.37</v>
       </c>
-      <c r="AB17" s="21">
+      <c r="AB17" s="13">
         <v>0</v>
       </c>
-      <c r="AC17" s="21">
+      <c r="AC17" s="13">
         <v>0.43</v>
       </c>
-      <c r="AD17" s="21">
+      <c r="AD17" s="13">
         <v>0.26</v>
       </c>
-      <c r="AE17" s="21">
+      <c r="AE17" s="13">
         <v>0.36</v>
       </c>
-      <c r="AF17" s="21">
+      <c r="AF17" s="13">
         <v>0.13</v>
       </c>
-      <c r="AG17" s="21">
+      <c r="AG17" s="13">
         <v>0.76</v>
       </c>
-      <c r="AH17" s="21">
+      <c r="AH17" s="13">
         <v>0.77</v>
       </c>
-      <c r="AI17" s="21">
+      <c r="AI17" s="13">
         <v>0.43</v>
       </c>
-      <c r="AJ17" s="21">
+      <c r="AJ17" s="13">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AK17" s="21">
+      <c r="AK17" s="13">
         <v>0.39</v>
       </c>
-      <c r="AL17" s="21">
+      <c r="AL17" s="13">
         <v>0.14000000000000001</v>
       </c>
-      <c r="AM17" s="21">
+      <c r="AM17" s="13">
         <v>0.96</v>
       </c>
-      <c r="AN17" s="21">
+      <c r="AN17" s="13">
         <v>0.86</v>
       </c>
     </row>
@@ -3284,103 +3321,103 @@
       <c r="G18">
         <v>119</v>
       </c>
-      <c r="H18" s="24">
+      <c r="H18" s="15">
         <v>0.35199999999999998</v>
       </c>
-      <c r="I18" s="29">
+      <c r="I18" s="19">
         <v>1</v>
       </c>
-      <c r="J18" s="29">
+      <c r="J18" s="19">
         <v>0.93</v>
       </c>
-      <c r="K18" s="29" t="s">
+      <c r="K18" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="L18" s="29">
+      <c r="L18" s="19">
         <v>100</v>
       </c>
-      <c r="M18" s="32">
+      <c r="M18" s="21">
         <v>0.34</v>
       </c>
-      <c r="N18" s="32">
+      <c r="N18" s="21">
         <v>0</v>
       </c>
-      <c r="O18" s="32" t="s">
+      <c r="O18" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="P18" s="32">
+      <c r="P18" s="21">
         <v>50</v>
       </c>
-      <c r="Q18" s="21">
+      <c r="Q18" s="13">
         <v>0.33</v>
       </c>
-      <c r="R18" s="21">
+      <c r="R18" s="13">
         <v>0.15</v>
       </c>
-      <c r="S18" s="21">
+      <c r="S18" s="13">
         <v>0.33</v>
       </c>
-      <c r="T18" s="21">
+      <c r="T18" s="13">
         <v>0.15</v>
       </c>
-      <c r="U18" s="21">
+      <c r="U18" s="13">
         <v>0.33</v>
       </c>
-      <c r="V18" s="21">
+      <c r="V18" s="13">
         <v>0.15</v>
       </c>
-      <c r="W18" s="21">
+      <c r="W18" s="13">
         <v>0.34</v>
       </c>
-      <c r="X18" s="21">
+      <c r="X18" s="13">
         <v>0</v>
       </c>
-      <c r="Y18" s="21">
+      <c r="Y18" s="13">
         <v>0.34</v>
       </c>
-      <c r="Z18" s="21">
+      <c r="Z18" s="13">
         <v>0</v>
       </c>
-      <c r="AA18" s="21">
+      <c r="AA18" s="13">
         <v>0.34</v>
       </c>
-      <c r="AB18" s="21">
+      <c r="AB18" s="13">
         <v>0</v>
       </c>
-      <c r="AC18" s="21">
+      <c r="AC18" s="13">
         <v>0.34</v>
       </c>
-      <c r="AD18" s="21">
+      <c r="AD18" s="13">
         <v>0.2</v>
       </c>
-      <c r="AE18" s="21">
+      <c r="AE18" s="13">
         <v>0.31</v>
       </c>
-      <c r="AF18" s="21">
+      <c r="AF18" s="13">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AG18" s="21">
+      <c r="AG18" s="13">
         <v>0.69</v>
       </c>
-      <c r="AH18" s="21">
+      <c r="AH18" s="13">
         <v>0.82</v>
       </c>
-      <c r="AI18" s="21">
+      <c r="AI18" s="13">
         <v>0.35</v>
       </c>
-      <c r="AJ18" s="21">
+      <c r="AJ18" s="13">
         <v>0.24</v>
       </c>
-      <c r="AK18" s="21">
+      <c r="AK18" s="13">
         <v>0.31</v>
       </c>
-      <c r="AL18" s="21">
+      <c r="AL18" s="13">
         <v>0.09</v>
       </c>
-      <c r="AM18" s="21">
+      <c r="AM18" s="13">
         <v>1</v>
       </c>
-      <c r="AN18" s="21">
+      <c r="AN18" s="13">
         <v>0.93</v>
       </c>
     </row>
@@ -3406,103 +3443,103 @@
       <c r="G19">
         <v>13</v>
       </c>
-      <c r="H19" s="24">
+      <c r="H19" s="15">
         <v>0.95499999999999996</v>
       </c>
-      <c r="I19" s="29">
+      <c r="I19" s="19">
         <v>1</v>
       </c>
-      <c r="J19" s="29">
+      <c r="J19" s="19">
         <v>0.11</v>
       </c>
-      <c r="K19" s="29" t="s">
+      <c r="K19" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="L19" s="29">
+      <c r="L19" s="19">
         <v>90</v>
       </c>
-      <c r="M19" s="32">
+      <c r="M19" s="21">
         <v>0.95</v>
       </c>
-      <c r="N19" s="32">
+      <c r="N19" s="21">
         <v>0.03</v>
       </c>
-      <c r="O19" s="32" t="s">
+      <c r="O19" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="P19" s="32">
+      <c r="P19" s="21">
         <v>50</v>
       </c>
-      <c r="Q19" s="21">
+      <c r="Q19" s="13">
         <v>0.92</v>
       </c>
-      <c r="R19" s="21">
+      <c r="R19" s="13">
         <v>0.05</v>
       </c>
-      <c r="S19" s="21">
+      <c r="S19" s="13">
         <v>0.92</v>
       </c>
-      <c r="T19" s="21">
+      <c r="T19" s="13">
         <v>0.05</v>
       </c>
-      <c r="U19" s="21">
+      <c r="U19" s="13">
         <v>0.92</v>
       </c>
-      <c r="V19" s="21">
+      <c r="V19" s="13">
         <v>0.05</v>
       </c>
-      <c r="W19" s="21">
+      <c r="W19" s="13">
         <v>0.95</v>
       </c>
-      <c r="X19" s="21">
+      <c r="X19" s="13">
         <v>0.03</v>
       </c>
-      <c r="Y19" s="21">
+      <c r="Y19" s="13">
         <v>0.95</v>
       </c>
-      <c r="Z19" s="21">
+      <c r="Z19" s="13">
         <v>0.03</v>
       </c>
-      <c r="AA19" s="21">
+      <c r="AA19" s="13">
         <v>0.95</v>
       </c>
-      <c r="AB19" s="21">
+      <c r="AB19" s="13">
         <v>0.03</v>
       </c>
-      <c r="AC19" s="21">
+      <c r="AC19" s="13">
         <v>0.97</v>
       </c>
-      <c r="AD19" s="21">
+      <c r="AD19" s="13">
         <v>0.09</v>
       </c>
-      <c r="AE19" s="21">
+      <c r="AE19" s="13">
         <v>0.97</v>
       </c>
-      <c r="AF19" s="21">
+      <c r="AF19" s="13">
         <v>0.09</v>
       </c>
-      <c r="AG19" s="21">
+      <c r="AG19" s="13">
         <v>1</v>
       </c>
-      <c r="AH19" s="21">
+      <c r="AH19" s="13">
         <v>0.11</v>
       </c>
-      <c r="AI19" s="21">
+      <c r="AI19" s="13">
         <v>0.95</v>
       </c>
-      <c r="AJ19" s="21">
+      <c r="AJ19" s="13">
         <v>0.09</v>
       </c>
-      <c r="AK19" s="21">
+      <c r="AK19" s="13">
         <v>0.95</v>
       </c>
-      <c r="AL19" s="21">
+      <c r="AL19" s="13">
         <v>0.09</v>
       </c>
-      <c r="AM19" s="21">
+      <c r="AM19" s="13">
         <v>1</v>
       </c>
-      <c r="AN19" s="21">
+      <c r="AN19" s="13">
         <v>0.12</v>
       </c>
     </row>
@@ -3528,103 +3565,103 @@
       <c r="G20">
         <v>18</v>
       </c>
-      <c r="H20" s="24">
+      <c r="H20" s="15">
         <v>0.97</v>
       </c>
-      <c r="I20" s="29">
+      <c r="I20" s="19">
         <v>0.98</v>
       </c>
-      <c r="J20" s="29">
+      <c r="J20" s="19">
         <v>0.19</v>
       </c>
-      <c r="K20" s="29" t="s">
+      <c r="K20" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="L20" s="29">
+      <c r="L20" s="19">
         <v>100</v>
       </c>
-      <c r="M20" s="32">
+      <c r="M20" s="21">
         <v>0.89</v>
       </c>
-      <c r="N20" s="32">
+      <c r="N20" s="21">
         <v>0.01</v>
       </c>
-      <c r="O20" s="32" t="s">
+      <c r="O20" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="P20" s="32">
+      <c r="P20" s="21">
         <v>50</v>
       </c>
-      <c r="Q20" s="21">
+      <c r="Q20" s="13">
         <v>0.92</v>
       </c>
-      <c r="R20" s="21">
+      <c r="R20" s="13">
         <v>0.09</v>
       </c>
-      <c r="S20" s="21">
+      <c r="S20" s="13">
         <v>0.92</v>
       </c>
-      <c r="T20" s="21">
+      <c r="T20" s="13">
         <v>0.09</v>
       </c>
-      <c r="U20" s="21">
+      <c r="U20" s="13">
         <v>0.92</v>
       </c>
-      <c r="V20" s="21">
+      <c r="V20" s="13">
         <v>0.09</v>
       </c>
-      <c r="W20" s="21">
+      <c r="W20" s="13">
         <v>0.89</v>
       </c>
-      <c r="X20" s="21">
+      <c r="X20" s="13">
         <v>0.01</v>
       </c>
-      <c r="Y20" s="21">
+      <c r="Y20" s="13">
         <v>0.89</v>
       </c>
-      <c r="Z20" s="21">
+      <c r="Z20" s="13">
         <v>0.01</v>
       </c>
-      <c r="AA20" s="21">
+      <c r="AA20" s="13">
         <v>0.89</v>
       </c>
-      <c r="AB20" s="21">
+      <c r="AB20" s="13">
         <v>0.01</v>
       </c>
-      <c r="AC20" s="21">
+      <c r="AC20" s="13">
         <v>0.89</v>
       </c>
-      <c r="AD20" s="21">
+      <c r="AD20" s="13">
         <v>0.06</v>
       </c>
-      <c r="AE20" s="21">
+      <c r="AE20" s="13">
         <v>0.89</v>
       </c>
-      <c r="AF20" s="21">
+      <c r="AF20" s="13">
         <v>0.06</v>
       </c>
-      <c r="AG20" s="21">
+      <c r="AG20" s="13">
         <v>0.95</v>
       </c>
-      <c r="AH20" s="21">
+      <c r="AH20" s="13">
         <v>0.15</v>
       </c>
-      <c r="AI20" s="21">
+      <c r="AI20" s="13">
         <v>0.89</v>
       </c>
-      <c r="AJ20" s="21">
+      <c r="AJ20" s="13">
         <v>0.08</v>
       </c>
-      <c r="AK20" s="21">
+      <c r="AK20" s="13">
         <v>0.89</v>
       </c>
-      <c r="AL20" s="21">
+      <c r="AL20" s="13">
         <v>0.08</v>
       </c>
-      <c r="AM20" s="21">
+      <c r="AM20" s="13">
         <v>0.98</v>
       </c>
-      <c r="AN20" s="21">
+      <c r="AN20" s="13">
         <v>0.19</v>
       </c>
     </row>
@@ -3650,103 +3687,103 @@
       <c r="G21">
         <v>18</v>
       </c>
-      <c r="H21" s="24">
+      <c r="H21" s="15">
         <v>0.94</v>
       </c>
-      <c r="I21" s="29">
+      <c r="I21" s="19">
         <v>0.98</v>
       </c>
-      <c r="J21" s="29">
+      <c r="J21" s="19">
         <v>0.25</v>
       </c>
-      <c r="K21" s="29" t="s">
+      <c r="K21" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="L21" s="29">
+      <c r="L21" s="19">
         <v>100</v>
       </c>
-      <c r="M21" s="32">
+      <c r="M21" s="21">
         <v>0.86</v>
       </c>
-      <c r="N21" s="32">
+      <c r="N21" s="21">
         <v>0.01</v>
       </c>
-      <c r="O21" s="32" t="s">
+      <c r="O21" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="P21" s="32">
+      <c r="P21" s="21">
         <v>50</v>
       </c>
-      <c r="Q21" s="21">
+      <c r="Q21" s="13">
         <v>0.91</v>
       </c>
-      <c r="R21" s="21">
+      <c r="R21" s="13">
         <v>0.14000000000000001</v>
       </c>
-      <c r="S21" s="21">
+      <c r="S21" s="13">
         <v>0.91</v>
       </c>
-      <c r="T21" s="21">
+      <c r="T21" s="13">
         <v>0.14000000000000001</v>
       </c>
-      <c r="U21" s="21">
+      <c r="U21" s="13">
         <v>0.91</v>
       </c>
-      <c r="V21" s="21">
+      <c r="V21" s="13">
         <v>0.14000000000000001</v>
       </c>
-      <c r="W21" s="21">
+      <c r="W21" s="13">
         <v>0.86</v>
       </c>
-      <c r="X21" s="21">
+      <c r="X21" s="13">
         <v>0.01</v>
       </c>
-      <c r="Y21" s="21">
+      <c r="Y21" s="13">
         <v>0.86</v>
       </c>
-      <c r="Z21" s="21">
+      <c r="Z21" s="13">
         <v>0.01</v>
       </c>
-      <c r="AA21" s="21">
+      <c r="AA21" s="13">
         <v>0.86</v>
       </c>
-      <c r="AB21" s="21">
+      <c r="AB21" s="13">
         <v>0.01</v>
       </c>
-      <c r="AC21" s="21">
+      <c r="AC21" s="13">
         <v>0.86</v>
       </c>
-      <c r="AD21" s="21">
+      <c r="AD21" s="13">
         <v>0.08</v>
       </c>
-      <c r="AE21" s="21">
+      <c r="AE21" s="13">
         <v>0.86</v>
       </c>
-      <c r="AF21" s="21">
+      <c r="AF21" s="13">
         <v>0.08</v>
       </c>
-      <c r="AG21" s="21">
+      <c r="AG21" s="13">
         <v>0.91</v>
       </c>
-      <c r="AH21" s="21">
+      <c r="AH21" s="13">
         <v>0.19</v>
       </c>
-      <c r="AI21" s="21">
+      <c r="AI21" s="13">
         <v>0.88</v>
       </c>
-      <c r="AJ21" s="21">
+      <c r="AJ21" s="13">
         <v>0.12</v>
       </c>
-      <c r="AK21" s="21">
+      <c r="AK21" s="13">
         <v>0.88</v>
       </c>
-      <c r="AL21" s="21">
+      <c r="AL21" s="13">
         <v>0.12</v>
       </c>
-      <c r="AM21" s="21">
+      <c r="AM21" s="13">
         <v>0.98</v>
       </c>
-      <c r="AN21" s="21">
+      <c r="AN21" s="13">
         <v>0.25</v>
       </c>
     </row>
@@ -3772,205 +3809,206 @@
       <c r="G22">
         <v>18</v>
       </c>
-      <c r="H22" s="25">
+      <c r="H22" s="16">
         <v>0.92500000000000004</v>
       </c>
-      <c r="I22" s="29">
+      <c r="I22" s="19">
         <v>0.98</v>
       </c>
-      <c r="J22" s="29">
+      <c r="J22" s="19">
         <v>0.28999999999999998</v>
       </c>
-      <c r="K22" s="29" t="s">
+      <c r="K22" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="L22" s="29">
+      <c r="L22" s="19">
         <v>100</v>
       </c>
-      <c r="M22" s="32">
+      <c r="M22" s="21">
         <v>0.83</v>
       </c>
-      <c r="N22" s="32">
+      <c r="N22" s="21">
         <v>0.01</v>
       </c>
-      <c r="O22" s="32" t="s">
+      <c r="O22" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="P22" s="32">
+      <c r="P22" s="21">
         <v>50</v>
       </c>
-      <c r="Q22" s="21">
+      <c r="Q22" s="13">
         <v>0.91</v>
       </c>
-      <c r="R22" s="21">
+      <c r="R22" s="13">
         <v>0.12</v>
       </c>
-      <c r="S22" s="21">
+      <c r="S22" s="13">
         <v>0.91</v>
       </c>
-      <c r="T22" s="21">
+      <c r="T22" s="13">
         <v>0.12</v>
       </c>
-      <c r="U22" s="21">
+      <c r="U22" s="13">
         <v>0.91</v>
       </c>
-      <c r="V22" s="21">
+      <c r="V22" s="13">
         <v>0.12</v>
       </c>
-      <c r="W22" s="21">
+      <c r="W22" s="13">
         <v>0.83</v>
       </c>
-      <c r="X22" s="21">
+      <c r="X22" s="13">
         <v>0.01</v>
       </c>
-      <c r="Y22" s="21">
+      <c r="Y22" s="13">
         <v>0.83</v>
       </c>
-      <c r="Z22" s="21">
+      <c r="Z22" s="13">
         <v>0.01</v>
       </c>
-      <c r="AA22" s="21">
+      <c r="AA22" s="13">
         <v>0.83</v>
       </c>
-      <c r="AB22" s="21">
+      <c r="AB22" s="13">
         <v>0.01</v>
       </c>
-      <c r="AC22" s="21">
+      <c r="AC22" s="13">
         <v>0.82</v>
       </c>
-      <c r="AD22" s="21">
+      <c r="AD22" s="13">
         <v>0.1</v>
       </c>
-      <c r="AE22" s="21">
+      <c r="AE22" s="13">
         <v>0.82</v>
       </c>
-      <c r="AF22" s="21">
+      <c r="AF22" s="13">
         <v>0.1</v>
       </c>
-      <c r="AG22" s="21">
+      <c r="AG22" s="13">
         <v>0.9</v>
       </c>
-      <c r="AH22" s="21">
+      <c r="AH22" s="13">
         <v>0.23</v>
       </c>
-      <c r="AI22" s="21">
+      <c r="AI22" s="13">
         <v>0.84</v>
       </c>
-      <c r="AJ22" s="21">
+      <c r="AJ22" s="13">
         <v>0.14000000000000001</v>
       </c>
-      <c r="AK22" s="21">
+      <c r="AK22" s="13">
         <v>0.84</v>
       </c>
-      <c r="AL22" s="21">
+      <c r="AL22" s="13">
         <v>0.14000000000000001</v>
       </c>
-      <c r="AM22" s="21">
+      <c r="AM22" s="13">
         <v>0.98</v>
       </c>
-      <c r="AN22" s="21">
+      <c r="AN22" s="13">
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:40" s="7" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+    <row r="23" spans="1:40" s="6" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="11">
+      <c r="D23" s="9">
         <v>315</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="6">
         <v>0.05</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="6">
         <v>4</v>
       </c>
-      <c r="H23" s="7">
+      <c r="H23" s="6">
         <v>0.69799999999999995</v>
       </c>
-      <c r="I23" s="26"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="26"/>
-      <c r="L23" s="26"/>
-      <c r="M23" s="26"/>
-      <c r="N23" s="26"/>
-      <c r="O23" s="26"/>
-      <c r="P23" s="26"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="17"/>
+      <c r="N23" s="17"/>
+      <c r="O23" s="17"/>
+      <c r="P23" s="17"/>
     </row>
-    <row r="24" spans="1:40" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+    <row r="24" spans="1:40" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="11">
+      <c r="D24" s="9">
         <v>185</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="6">
         <v>0.1</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F24" s="6">
         <v>4</v>
       </c>
-      <c r="H24" s="7">
+      <c r="H24" s="6">
         <v>0.66400000000000003</v>
       </c>
     </row>
-    <row r="25" spans="1:40" s="7" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
+    <row r="25" spans="1:40" s="6" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D25" s="9">
         <v>142</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="6">
         <v>0.15</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="6">
         <v>4</v>
       </c>
-      <c r="H25" s="7">
+      <c r="H25" s="6">
         <v>0.65300000000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:40" s="7" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+    <row r="26" spans="1:40" s="6" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D26" s="11">
+      <c r="D26" s="9">
         <v>126</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="6">
         <v>0.2</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F26" s="6">
         <v>4</v>
       </c>
-      <c r="H26" s="7">
+      <c r="H26" s="6">
         <v>0.61599999999999999</v>
       </c>
+      <c r="I26" s="35"/>
     </row>
     <row r="27" spans="1:40" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -3994,17 +4032,105 @@
       <c r="G27">
         <v>1080</v>
       </c>
-      <c r="H27" s="9">
+      <c r="H27" s="33">
         <v>0.35299999999999998</v>
       </c>
-      <c r="I27" s="29"/>
-      <c r="J27" s="29"/>
-      <c r="K27" s="29"/>
-      <c r="L27" s="29"/>
-      <c r="M27" s="32"/>
-      <c r="N27" s="32"/>
-      <c r="O27" s="32"/>
-      <c r="P27" s="32"/>
+      <c r="I27" s="31">
+        <v>0.01</v>
+      </c>
+      <c r="J27" s="34">
+        <v>0.33</v>
+      </c>
+      <c r="K27" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="L27" s="31">
+        <v>90</v>
+      </c>
+      <c r="M27" s="32">
+        <v>0</v>
+      </c>
+      <c r="N27" s="32">
+        <v>0.13</v>
+      </c>
+      <c r="O27" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="P27" s="32">
+        <v>50</v>
+      </c>
+      <c r="Q27" s="30">
+        <v>-0.01</v>
+      </c>
+      <c r="R27" s="30">
+        <v>0.38</v>
+      </c>
+      <c r="S27" s="30">
+        <v>-0.01</v>
+      </c>
+      <c r="T27" s="30">
+        <v>0.37</v>
+      </c>
+      <c r="U27" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="V27" s="30">
+        <v>1</v>
+      </c>
+      <c r="W27" s="30">
+        <v>0</v>
+      </c>
+      <c r="X27" s="30">
+        <v>0.13</v>
+      </c>
+      <c r="Y27" s="30">
+        <v>0</v>
+      </c>
+      <c r="Z27" s="30">
+        <v>0.13</v>
+      </c>
+      <c r="AA27" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB27" s="30">
+        <v>1</v>
+      </c>
+      <c r="AC27" s="30">
+        <v>0.01</v>
+      </c>
+      <c r="AD27" s="30">
+        <v>0.33</v>
+      </c>
+      <c r="AE27" s="30">
+        <v>0</v>
+      </c>
+      <c r="AF27" s="30">
+        <v>0.66</v>
+      </c>
+      <c r="AG27" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH27" s="30">
+        <v>1</v>
+      </c>
+      <c r="AI27" s="30">
+        <v>0</v>
+      </c>
+      <c r="AJ27" s="30">
+        <v>0.36</v>
+      </c>
+      <c r="AK27" s="30">
+        <v>-0.01</v>
+      </c>
+      <c r="AL27" s="30">
+        <v>0.72</v>
+      </c>
+      <c r="AM27" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="AN27" s="30">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:40" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -4028,17 +4154,105 @@
       <c r="G28">
         <v>1080</v>
       </c>
-      <c r="H28" s="6">
+      <c r="H28" s="15">
         <v>0.48</v>
       </c>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
-      <c r="K28" s="29"/>
-      <c r="L28" s="29"/>
-      <c r="M28" s="32"/>
-      <c r="N28" s="32"/>
-      <c r="O28" s="32"/>
-      <c r="P28" s="32"/>
+      <c r="I28" s="31">
+        <v>0.01</v>
+      </c>
+      <c r="J28" s="34">
+        <v>0.09</v>
+      </c>
+      <c r="K28" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="L28" s="31">
+        <v>90</v>
+      </c>
+      <c r="M28" s="32">
+        <v>-0.01</v>
+      </c>
+      <c r="N28" s="32">
+        <v>0.01</v>
+      </c>
+      <c r="O28" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="P28" s="32">
+        <v>50</v>
+      </c>
+      <c r="Q28" s="30">
+        <v>-0.01</v>
+      </c>
+      <c r="R28" s="30">
+        <v>0.47</v>
+      </c>
+      <c r="S28" s="30">
+        <v>-0.01</v>
+      </c>
+      <c r="T28" s="30">
+        <v>0.45</v>
+      </c>
+      <c r="U28" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="V28" s="30">
+        <v>1</v>
+      </c>
+      <c r="W28" s="30">
+        <v>-0.01</v>
+      </c>
+      <c r="X28" s="30">
+        <v>0.01</v>
+      </c>
+      <c r="Y28" s="30">
+        <v>-0.01</v>
+      </c>
+      <c r="Z28" s="30">
+        <v>0.01</v>
+      </c>
+      <c r="AA28" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB28" s="30">
+        <v>1</v>
+      </c>
+      <c r="AC28" s="30">
+        <v>0.01</v>
+      </c>
+      <c r="AD28" s="30">
+        <v>0.09</v>
+      </c>
+      <c r="AE28" s="30">
+        <v>-0.01</v>
+      </c>
+      <c r="AF28" s="30">
+        <v>0.88</v>
+      </c>
+      <c r="AG28" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH28" s="30">
+        <v>1</v>
+      </c>
+      <c r="AI28" s="30">
+        <v>0</v>
+      </c>
+      <c r="AJ28" s="30">
+        <v>0.11</v>
+      </c>
+      <c r="AK28" s="30">
+        <v>-0.01</v>
+      </c>
+      <c r="AL28" s="30">
+        <v>0.94</v>
+      </c>
+      <c r="AM28" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="AN28" s="30">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -4062,17 +4276,105 @@
       <c r="G29">
         <v>1080</v>
       </c>
-      <c r="H29" s="6">
+      <c r="H29" s="15">
         <v>0.5</v>
       </c>
-      <c r="I29" s="29"/>
-      <c r="J29" s="29"/>
-      <c r="K29" s="29"/>
-      <c r="L29" s="29"/>
-      <c r="M29" s="32"/>
-      <c r="N29" s="32"/>
-      <c r="O29" s="32"/>
-      <c r="P29" s="32"/>
+      <c r="I29" s="31">
+        <v>0.04</v>
+      </c>
+      <c r="J29" s="34">
+        <v>0.27</v>
+      </c>
+      <c r="K29" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="L29" s="31">
+        <v>25</v>
+      </c>
+      <c r="M29" s="32">
+        <v>0.03</v>
+      </c>
+      <c r="N29" s="32">
+        <v>0</v>
+      </c>
+      <c r="O29" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="P29" s="32">
+        <v>50</v>
+      </c>
+      <c r="Q29" s="30">
+        <v>0.04</v>
+      </c>
+      <c r="R29" s="30">
+        <v>0.27</v>
+      </c>
+      <c r="S29" s="30">
+        <v>0.04</v>
+      </c>
+      <c r="T29" s="30">
+        <v>0.24</v>
+      </c>
+      <c r="U29" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="V29" s="30">
+        <v>1</v>
+      </c>
+      <c r="W29" s="30">
+        <v>0.03</v>
+      </c>
+      <c r="X29" s="30">
+        <v>0</v>
+      </c>
+      <c r="Y29" s="30">
+        <v>0.03</v>
+      </c>
+      <c r="Z29" s="30">
+        <v>0</v>
+      </c>
+      <c r="AA29" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB29" s="30">
+        <v>1</v>
+      </c>
+      <c r="AC29" s="30">
+        <v>-0.01</v>
+      </c>
+      <c r="AD29" s="30">
+        <v>0.02</v>
+      </c>
+      <c r="AE29" s="30">
+        <v>-0.02</v>
+      </c>
+      <c r="AF29" s="30">
+        <v>0.98</v>
+      </c>
+      <c r="AG29" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH29" s="30">
+        <v>1</v>
+      </c>
+      <c r="AI29" s="30">
+        <v>0.01</v>
+      </c>
+      <c r="AJ29" s="30">
+        <v>0.02</v>
+      </c>
+      <c r="AK29" s="30">
+        <v>-0.02</v>
+      </c>
+      <c r="AL29" s="30">
+        <v>0.99</v>
+      </c>
+      <c r="AM29" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="AN29" s="30">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:40" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -4096,112 +4398,112 @@
       <c r="G30">
         <v>1080</v>
       </c>
-      <c r="H30" s="8">
+      <c r="H30" s="7">
         <v>0.47199999999999998</v>
       </c>
-      <c r="I30" s="29"/>
-      <c r="J30" s="29"/>
-      <c r="K30" s="29"/>
-      <c r="L30" s="29"/>
-      <c r="M30" s="32"/>
-      <c r="N30" s="32"/>
-      <c r="O30" s="32"/>
-      <c r="P30" s="32"/>
+      <c r="I30" s="36"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="19"/>
+      <c r="L30" s="19"/>
+      <c r="M30" s="21"/>
+      <c r="N30" s="21"/>
+      <c r="O30" s="21"/>
+      <c r="P30" s="21"/>
     </row>
-    <row r="31" spans="1:40" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
+    <row r="31" spans="1:40" s="6" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C31" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="11">
+      <c r="D31" s="9">
         <v>267</v>
       </c>
-      <c r="E31" s="7">
+      <c r="E31" s="6">
         <v>0.01</v>
       </c>
-      <c r="F31" s="7">
+      <c r="F31" s="6">
         <v>4</v>
       </c>
-      <c r="H31" s="7">
+      <c r="H31" s="6">
         <v>0.44900000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:40" s="7" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
+    <row r="32" spans="1:40" s="6" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C32" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D32" s="11">
+      <c r="D32" s="9">
         <v>95</v>
       </c>
-      <c r="E32" s="7">
+      <c r="E32" s="6">
         <v>0.04</v>
       </c>
-      <c r="F32" s="7">
+      <c r="F32" s="6">
         <v>4</v>
       </c>
-      <c r="H32" s="7">
+      <c r="H32" s="6">
         <v>0.31900000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="7" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
+    <row r="33" spans="1:8" s="6" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D33" s="11">
+      <c r="D33" s="9">
         <v>64</v>
       </c>
-      <c r="E33" s="7">
+      <c r="E33" s="6">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F33" s="7">
+      <c r="F33" s="6">
         <v>4</v>
       </c>
-      <c r="H33" s="7">
+      <c r="H33" s="6">
         <v>0.24099999999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="7" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
+    <row r="34" spans="1:8" s="6" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D34" s="11">
+      <c r="D34" s="9">
         <v>44</v>
       </c>
-      <c r="E34" s="7">
+      <c r="E34" s="6">
         <v>0.1</v>
       </c>
-      <c r="F34" s="7">
+      <c r="F34" s="6">
         <v>4</v>
       </c>
-      <c r="H34" s="7">
+      <c r="H34" s="6">
         <v>0.23400000000000001</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H35" s="12"/>
+      <c r="H35" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="21">

</xml_diff>

<commit_message>
Code with graphs before removing graphics logics.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tudublin-my.sharepoint.com/personal/lucas_rizzo_tudublin_ie/Documents/rulex/Multiclass/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="691" documentId="11_AD4DB114E441178AC67DF4065653DB7A683EDF12" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0D6743E-6A2D-47FD-9E22-9517CCF1BE9E}"/>
+  <xr:revisionPtr revIDLastSave="697" documentId="11_AD4DB114E441178AC67DF4065653DB7A683EDF12" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03701944-C317-4FF4-A465-5896BA7093BB}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="54">
   <si>
     <t>Data</t>
   </si>
@@ -238,6 +238,12 @@
   </si>
   <si>
     <t>nan</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>g+K3:K22rounded</t>
   </si>
 </sst>
 </file>
@@ -519,20 +525,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -543,13 +550,12 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1227,9 +1233,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O22" sqref="M15:O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1276,99 +1282,99 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="32" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="I1" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="29" t="s">
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="24" t="s">
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
+      <c r="Q1" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="R1" s="24"/>
-      <c r="S1" s="22" t="s">
+      <c r="R1" s="30"/>
+      <c r="S1" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="T1" s="24"/>
-      <c r="U1" s="22" t="s">
+      <c r="T1" s="30"/>
+      <c r="U1" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="V1" s="23"/>
-      <c r="W1" s="22" t="s">
+      <c r="V1" s="31"/>
+      <c r="W1" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="X1" s="24"/>
-      <c r="Y1" s="22" t="s">
+      <c r="X1" s="30"/>
+      <c r="Y1" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="Z1" s="24"/>
-      <c r="AA1" s="22" t="s">
+      <c r="Z1" s="30"/>
+      <c r="AA1" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="23"/>
-      <c r="AC1" s="22" t="s">
+      <c r="AB1" s="31"/>
+      <c r="AC1" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="24"/>
-      <c r="AE1" s="22" t="s">
+      <c r="AD1" s="30"/>
+      <c r="AE1" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="AF1" s="24"/>
-      <c r="AG1" s="22" t="s">
+      <c r="AF1" s="30"/>
+      <c r="AG1" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="AH1" s="23"/>
-      <c r="AI1" s="22" t="s">
+      <c r="AH1" s="31"/>
+      <c r="AI1" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="AJ1" s="24"/>
-      <c r="AK1" s="22" t="s">
+      <c r="AJ1" s="30"/>
+      <c r="AK1" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="AL1" s="24"/>
-      <c r="AM1" s="22" t="s">
+      <c r="AL1" s="30"/>
+      <c r="AM1" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="AN1" s="23"/>
+      <c r="AN1" s="31"/>
     </row>
     <row r="2" spans="1:40" s="3" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="27"/>
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="32"/>
       <c r="H2" s="14" t="s">
         <v>5</v>
       </c>
@@ -1501,7 +1507,7 @@
         <v>0.26</v>
       </c>
       <c r="K3" s="19" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="L3" s="19">
         <v>100</v>
@@ -4008,7 +4014,7 @@
       <c r="H26" s="6">
         <v>0.61599999999999999</v>
       </c>
-      <c r="I26" s="35"/>
+      <c r="I26" s="27"/>
     </row>
     <row r="27" spans="1:40" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -4018,7 +4024,7 @@
         <v>36</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="D27">
         <v>48</v>
@@ -4032,103 +4038,103 @@
       <c r="G27">
         <v>1080</v>
       </c>
-      <c r="H27" s="33">
+      <c r="H27" s="25">
         <v>0.35299999999999998</v>
       </c>
-      <c r="I27" s="31">
+      <c r="I27" s="23">
         <v>0.01</v>
       </c>
-      <c r="J27" s="34">
+      <c r="J27" s="26">
         <v>0.33</v>
       </c>
-      <c r="K27" s="31" t="s">
+      <c r="K27" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="L27" s="31">
+      <c r="L27" s="23">
         <v>90</v>
       </c>
-      <c r="M27" s="32">
+      <c r="M27" s="24">
         <v>0</v>
       </c>
-      <c r="N27" s="32">
+      <c r="N27" s="24">
         <v>0.13</v>
       </c>
-      <c r="O27" s="32" t="s">
+      <c r="O27" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="P27" s="32">
+      <c r="P27" s="24">
         <v>50</v>
       </c>
-      <c r="Q27" s="30">
+      <c r="Q27" s="22">
         <v>-0.01</v>
       </c>
-      <c r="R27" s="30">
+      <c r="R27" s="22">
         <v>0.38</v>
       </c>
-      <c r="S27" s="30">
+      <c r="S27" s="22">
         <v>-0.01</v>
       </c>
-      <c r="T27" s="30">
+      <c r="T27" s="22">
         <v>0.37</v>
       </c>
-      <c r="U27" s="30" t="s">
+      <c r="U27" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="V27" s="30">
+      <c r="V27" s="22">
         <v>1</v>
       </c>
-      <c r="W27" s="30">
+      <c r="W27" s="22">
         <v>0</v>
       </c>
-      <c r="X27" s="30">
+      <c r="X27" s="22">
         <v>0.13</v>
       </c>
-      <c r="Y27" s="30">
+      <c r="Y27" s="22">
         <v>0</v>
       </c>
-      <c r="Z27" s="30">
+      <c r="Z27" s="22">
         <v>0.13</v>
       </c>
-      <c r="AA27" s="30" t="s">
+      <c r="AA27" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="AB27" s="30">
+      <c r="AB27" s="22">
         <v>1</v>
       </c>
-      <c r="AC27" s="30">
+      <c r="AC27" s="22">
         <v>0.01</v>
       </c>
-      <c r="AD27" s="30">
+      <c r="AD27" s="22">
         <v>0.33</v>
       </c>
-      <c r="AE27" s="30">
+      <c r="AE27" s="22">
         <v>0</v>
       </c>
-      <c r="AF27" s="30">
+      <c r="AF27" s="22">
         <v>0.66</v>
       </c>
-      <c r="AG27" s="30" t="s">
+      <c r="AG27" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="AH27" s="30">
+      <c r="AH27" s="22">
         <v>1</v>
       </c>
-      <c r="AI27" s="30">
+      <c r="AI27" s="22">
         <v>0</v>
       </c>
-      <c r="AJ27" s="30">
+      <c r="AJ27" s="22">
         <v>0.36</v>
       </c>
-      <c r="AK27" s="30">
+      <c r="AK27" s="22">
         <v>-0.01</v>
       </c>
-      <c r="AL27" s="30">
+      <c r="AL27" s="22">
         <v>0.72</v>
       </c>
-      <c r="AM27" s="30" t="s">
+      <c r="AM27" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="AN27" s="30">
+      <c r="AN27" s="22">
         <v>1</v>
       </c>
     </row>
@@ -4157,100 +4163,100 @@
       <c r="H28" s="15">
         <v>0.48</v>
       </c>
-      <c r="I28" s="31">
+      <c r="I28" s="23">
         <v>0.01</v>
       </c>
-      <c r="J28" s="34">
+      <c r="J28" s="26">
         <v>0.09</v>
       </c>
-      <c r="K28" s="31" t="s">
+      <c r="K28" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="L28" s="31">
+      <c r="L28" s="23">
         <v>90</v>
       </c>
-      <c r="M28" s="32">
+      <c r="M28" s="24">
         <v>-0.01</v>
       </c>
-      <c r="N28" s="32">
+      <c r="N28" s="24">
         <v>0.01</v>
       </c>
-      <c r="O28" s="32" t="s">
+      <c r="O28" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="P28" s="32">
+      <c r="P28" s="24">
         <v>50</v>
       </c>
-      <c r="Q28" s="30">
+      <c r="Q28" s="22">
         <v>-0.01</v>
       </c>
-      <c r="R28" s="30">
+      <c r="R28" s="22">
         <v>0.47</v>
       </c>
-      <c r="S28" s="30">
+      <c r="S28" s="22">
         <v>-0.01</v>
       </c>
-      <c r="T28" s="30">
+      <c r="T28" s="22">
         <v>0.45</v>
       </c>
-      <c r="U28" s="30" t="s">
+      <c r="U28" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="V28" s="30">
+      <c r="V28" s="22">
         <v>1</v>
       </c>
-      <c r="W28" s="30">
+      <c r="W28" s="22">
         <v>-0.01</v>
       </c>
-      <c r="X28" s="30">
+      <c r="X28" s="22">
         <v>0.01</v>
       </c>
-      <c r="Y28" s="30">
+      <c r="Y28" s="22">
         <v>-0.01</v>
       </c>
-      <c r="Z28" s="30">
+      <c r="Z28" s="22">
         <v>0.01</v>
       </c>
-      <c r="AA28" s="30" t="s">
+      <c r="AA28" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="AB28" s="30">
+      <c r="AB28" s="22">
         <v>1</v>
       </c>
-      <c r="AC28" s="30">
+      <c r="AC28" s="22">
         <v>0.01</v>
       </c>
-      <c r="AD28" s="30">
+      <c r="AD28" s="22">
         <v>0.09</v>
       </c>
-      <c r="AE28" s="30">
+      <c r="AE28" s="22">
         <v>-0.01</v>
       </c>
-      <c r="AF28" s="30">
+      <c r="AF28" s="22">
         <v>0.88</v>
       </c>
-      <c r="AG28" s="30" t="s">
+      <c r="AG28" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="AH28" s="30">
+      <c r="AH28" s="22">
         <v>1</v>
       </c>
-      <c r="AI28" s="30">
+      <c r="AI28" s="22">
         <v>0</v>
       </c>
-      <c r="AJ28" s="30">
+      <c r="AJ28" s="22">
         <v>0.11</v>
       </c>
-      <c r="AK28" s="30">
+      <c r="AK28" s="22">
         <v>-0.01</v>
       </c>
-      <c r="AL28" s="30">
+      <c r="AL28" s="22">
         <v>0.94</v>
       </c>
-      <c r="AM28" s="30" t="s">
+      <c r="AM28" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="AN28" s="30">
+      <c r="AN28" s="22">
         <v>1</v>
       </c>
     </row>
@@ -4279,100 +4285,100 @@
       <c r="H29" s="15">
         <v>0.5</v>
       </c>
-      <c r="I29" s="31">
+      <c r="I29" s="23">
         <v>0.04</v>
       </c>
-      <c r="J29" s="34">
+      <c r="J29" s="26">
         <v>0.27</v>
       </c>
-      <c r="K29" s="31" t="s">
+      <c r="K29" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="L29" s="31">
+      <c r="L29" s="23">
         <v>25</v>
       </c>
-      <c r="M29" s="32">
+      <c r="M29" s="24">
         <v>0.03</v>
       </c>
-      <c r="N29" s="32">
+      <c r="N29" s="24">
         <v>0</v>
       </c>
-      <c r="O29" s="32" t="s">
+      <c r="O29" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="P29" s="32">
+      <c r="P29" s="24">
         <v>50</v>
       </c>
-      <c r="Q29" s="30">
+      <c r="Q29" s="22">
         <v>0.04</v>
       </c>
-      <c r="R29" s="30">
+      <c r="R29" s="22">
         <v>0.27</v>
       </c>
-      <c r="S29" s="30">
+      <c r="S29" s="22">
         <v>0.04</v>
       </c>
-      <c r="T29" s="30">
+      <c r="T29" s="22">
         <v>0.24</v>
       </c>
-      <c r="U29" s="30" t="s">
+      <c r="U29" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="V29" s="30">
+      <c r="V29" s="22">
         <v>1</v>
       </c>
-      <c r="W29" s="30">
+      <c r="W29" s="22">
         <v>0.03</v>
       </c>
-      <c r="X29" s="30">
+      <c r="X29" s="22">
         <v>0</v>
       </c>
-      <c r="Y29" s="30">
+      <c r="Y29" s="22">
         <v>0.03</v>
       </c>
-      <c r="Z29" s="30">
+      <c r="Z29" s="22">
         <v>0</v>
       </c>
-      <c r="AA29" s="30" t="s">
+      <c r="AA29" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="AB29" s="30">
+      <c r="AB29" s="22">
         <v>1</v>
       </c>
-      <c r="AC29" s="30">
+      <c r="AC29" s="22">
         <v>-0.01</v>
       </c>
-      <c r="AD29" s="30">
+      <c r="AD29" s="22">
         <v>0.02</v>
       </c>
-      <c r="AE29" s="30">
+      <c r="AE29" s="22">
         <v>-0.02</v>
       </c>
-      <c r="AF29" s="30">
+      <c r="AF29" s="22">
         <v>0.98</v>
       </c>
-      <c r="AG29" s="30" t="s">
+      <c r="AG29" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="AH29" s="30">
+      <c r="AH29" s="22">
         <v>1</v>
       </c>
-      <c r="AI29" s="30">
+      <c r="AI29" s="22">
         <v>0.01</v>
       </c>
-      <c r="AJ29" s="30">
+      <c r="AJ29" s="22">
         <v>0.02</v>
       </c>
-      <c r="AK29" s="30">
+      <c r="AK29" s="22">
         <v>-0.02</v>
       </c>
-      <c r="AL29" s="30">
+      <c r="AL29" s="22">
         <v>0.99</v>
       </c>
-      <c r="AM29" s="30" t="s">
+      <c r="AM29" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="AN29" s="30">
+      <c r="AN29" s="22">
         <v>1</v>
       </c>
     </row>
@@ -4401,7 +4407,7 @@
       <c r="H30" s="7">
         <v>0.47199999999999998</v>
       </c>
-      <c r="I30" s="36"/>
+      <c r="I30" s="28"/>
       <c r="J30" s="19"/>
       <c r="K30" s="19"/>
       <c r="L30" s="19"/>
@@ -4507,6 +4513,20 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="AM1:AN1"/>
+    <mergeCell ref="AA1:AB1"/>
+    <mergeCell ref="AC1:AD1"/>
+    <mergeCell ref="AE1:AF1"/>
+    <mergeCell ref="AG1:AH1"/>
+    <mergeCell ref="AI1:AJ1"/>
+    <mergeCell ref="AK1:AL1"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="Y1:Z1"/>
     <mergeCell ref="Q1:R1"/>
     <mergeCell ref="S1:T1"/>
@@ -4514,20 +4534,6 @@
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="I1:L1"/>
     <mergeCell ref="M1:P1"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="W1:X1"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="AM1:AN1"/>
-    <mergeCell ref="AA1:AB1"/>
-    <mergeCell ref="AC1:AD1"/>
-    <mergeCell ref="AE1:AF1"/>
-    <mergeCell ref="AG1:AH1"/>
-    <mergeCell ref="AI1:AJ1"/>
-    <mergeCell ref="AK1:AL1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4538,7 +4544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F773C87-B1CB-4300-9A68-CEC548FE408C}">
   <dimension ref="A3:AB32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>

</xml_diff>